<commit_message>
2025-10-09 update by pms
navMesh추가
몬스터 추락시 deadZone Trigger추가
</commit_message>
<xml_diff>
--- a/Table/ResourceTable.xlsx
+++ b/Table/ResourceTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Project\Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEE6409-903A-405E-BBEB-AF281811814C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDE1B70-84B1-4AAB-8B1F-81765529B7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" tabRatio="714" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2175" yWindow="2175" windowWidth="21600" windowHeight="11332" tabRatio="714" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resource" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Id</t>
   </si>
@@ -165,6 +165,9 @@
   <si>
     <t>Map/Obstacles</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MapTileDeadZone</t>
   </si>
 </sst>
 </file>
@@ -355,16 +358,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2252,10 +2255,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:O1506"/>
+  <dimension ref="A2:O1507"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -2314,7 +2317,7 @@
       <c r="F4" s="2">
         <v>1</v>
       </c>
-      <c r="H4" s="12"/>
+      <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A5" s="13"/>
@@ -2331,7 +2334,7 @@
       <c r="F5" s="2">
         <v>1</v>
       </c>
-      <c r="H5" s="12"/>
+      <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A6" s="13"/>
@@ -2347,48 +2350,48 @@
       <c r="F6" s="2">
         <v>1</v>
       </c>
-      <c r="H6" s="12"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A7" s="13"/>
       <c r="C7" s="9">
+        <v>103</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A8" s="13"/>
+      <c r="C8" s="9">
         <v>1001</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E8" s="2">
         <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A8" s="13"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9">
-        <v>1005</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
       </c>
-      <c r="H8" s="12"/>
+      <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A9" s="13"/>
-      <c r="C9" s="2">
-        <v>1011</v>
+      <c r="B9" s="10"/>
+      <c r="C9" s="9">
+        <v>1005</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="2">
         <v>1</v>
@@ -2396,16 +2399,15 @@
       <c r="F9" s="2">
         <v>0</v>
       </c>
-      <c r="H9" s="12"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A10" s="13"/>
-      <c r="B10" s="10"/>
       <c r="C10" s="2">
-        <v>1012</v>
+        <v>1011</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>27</v>
+      <c r="D10" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
@@ -2413,16 +2415,16 @@
       <c r="F10" s="2">
         <v>0</v>
       </c>
-      <c r="H10" s="9"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A11" s="13"/>
       <c r="B11" s="10"/>
       <c r="C11" s="2">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" s="2">
         <v>1</v>
@@ -2436,10 +2438,10 @@
       <c r="A12" s="13"/>
       <c r="B12" s="10"/>
       <c r="C12" s="2">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
@@ -2452,12 +2454,24 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A13" s="13"/>
       <c r="B13" s="10"/>
-      <c r="G13" s="11"/>
+      <c r="C13" s="2">
+        <v>1014</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
       <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A14" s="13"/>
       <c r="B14" s="10"/>
+      <c r="G14" s="11"/>
       <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.6">
@@ -2478,78 +2492,78 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A18" s="13"/>
       <c r="B18" s="10"/>
-      <c r="H18" s="12"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A19" s="13"/>
       <c r="B19" s="10"/>
-      <c r="H19" s="12"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A20" s="13"/>
       <c r="B20" s="10"/>
-      <c r="H20" s="12"/>
+      <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A21" s="13"/>
       <c r="B21" s="10"/>
-      <c r="H21" s="12"/>
+      <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A22" s="13"/>
       <c r="B22" s="10"/>
-      <c r="H22" s="12"/>
+      <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A23" s="13"/>
       <c r="B23" s="10"/>
-      <c r="H23" s="12"/>
+      <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A24" s="13"/>
       <c r="B24" s="10"/>
-      <c r="H24" s="12"/>
+      <c r="H24" s="14"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A25" s="13"/>
       <c r="B25" s="10"/>
-      <c r="H25" s="12"/>
+      <c r="H25" s="14"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A26" s="13"/>
       <c r="B26" s="10"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="12"/>
+      <c r="H26" s="14"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A27" s="13"/>
       <c r="B27" s="10"/>
-      <c r="H27" s="12"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="14"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A28" s="13"/>
       <c r="B28" s="10"/>
-      <c r="H28" s="12"/>
+      <c r="H28" s="14"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A29" s="13"/>
       <c r="B29" s="10"/>
-      <c r="H29" s="12"/>
+      <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A30" s="13"/>
       <c r="B30" s="10"/>
-      <c r="H30" s="12"/>
+      <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A31" s="13"/>
       <c r="B31" s="10"/>
-      <c r="H31" s="12"/>
+      <c r="H31" s="14"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A32" s="13"/>
       <c r="B32" s="10"/>
-      <c r="H32" s="9"/>
+      <c r="H32" s="14"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A33" s="13"/>
@@ -2574,32 +2588,32 @@
     <row r="37" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A37" s="13"/>
       <c r="B37" s="10"/>
-      <c r="H37" s="12"/>
+      <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A38" s="13"/>
       <c r="B38" s="10"/>
-      <c r="H38" s="12"/>
+      <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A39" s="13"/>
       <c r="B39" s="10"/>
-      <c r="H39" s="12"/>
+      <c r="H39" s="14"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A40" s="13"/>
       <c r="B40" s="10"/>
-      <c r="H40" s="12"/>
+      <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A41" s="13"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="12"/>
+      <c r="B41" s="10"/>
+      <c r="H41" s="14"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-      <c r="H42" s="9"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="14"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A43" s="13"/>
@@ -2640,624 +2654,619 @@
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="H50" s="9"/>
-      <c r="I50" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J50" s="12"/>
-      <c r="K50" s="12"/>
-      <c r="L50" s="12"/>
-      <c r="M50" s="12"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="H51" s="9"/>
-      <c r="I51" s="12"/>
-      <c r="J51" s="12"/>
-      <c r="K51" s="12"/>
-      <c r="L51" s="12"/>
-      <c r="M51" s="12"/>
+      <c r="I51" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="14"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
-      <c r="D52" s="5"/>
       <c r="H52" s="9"/>
-      <c r="I52" s="12"/>
-      <c r="J52" s="12"/>
-      <c r="K52" s="12"/>
-      <c r="L52" s="12"/>
-      <c r="M52" s="12"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="14"/>
+      <c r="M52" s="14"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
+      <c r="D53" s="5"/>
       <c r="H53" s="9"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12"/>
-      <c r="K53" s="12"/>
-      <c r="L53" s="12"/>
-      <c r="M53" s="12"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="14"/>
+      <c r="L53" s="14"/>
+      <c r="M53" s="14"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="H54" s="9"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="12"/>
-      <c r="K54" s="12"/>
-      <c r="L54" s="12"/>
-      <c r="M54" s="12"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="14"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="H55" s="9"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="12"/>
-      <c r="K55" s="12"/>
-      <c r="L55" s="12"/>
-      <c r="M55" s="12"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="14"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="H56" s="9"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
-      <c r="K56" s="12"/>
-      <c r="L56" s="12"/>
-      <c r="M56" s="12"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+      <c r="K56" s="14"/>
+      <c r="L56" s="14"/>
+      <c r="M56" s="14"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="H57" s="9"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="12"/>
-      <c r="K57" s="12"/>
-      <c r="L57" s="12"/>
-      <c r="M57" s="12"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="14"/>
+      <c r="L57" s="14"/>
+      <c r="M57" s="14"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="H58" s="9"/>
-      <c r="I58" s="12"/>
-      <c r="J58" s="12"/>
-      <c r="K58" s="12"/>
-      <c r="L58" s="12"/>
-      <c r="M58" s="12"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="14"/>
+      <c r="L58" s="14"/>
+      <c r="M58" s="14"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="H59" s="9"/>
-      <c r="I59" s="12"/>
-      <c r="J59" s="12"/>
-      <c r="K59" s="12"/>
-      <c r="L59" s="12"/>
-      <c r="M59" s="12"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="14"/>
+      <c r="K59" s="14"/>
+      <c r="L59" s="14"/>
+      <c r="M59" s="14"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="H60" s="9"/>
-      <c r="I60" s="12"/>
-      <c r="J60" s="12"/>
-      <c r="K60" s="12"/>
-      <c r="L60" s="12"/>
-      <c r="M60" s="12"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="14"/>
+      <c r="K60" s="14"/>
+      <c r="L60" s="14"/>
+      <c r="M60" s="14"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
       <c r="H61" s="9"/>
-      <c r="I61" s="12"/>
-      <c r="J61" s="12"/>
-      <c r="K61" s="12"/>
-      <c r="L61" s="12"/>
-      <c r="M61" s="12"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="14"/>
+      <c r="K61" s="14"/>
+      <c r="L61" s="14"/>
+      <c r="M61" s="14"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="H62" s="9"/>
-      <c r="I62" s="12"/>
-      <c r="J62" s="12"/>
-      <c r="K62" s="12"/>
-      <c r="L62" s="12"/>
-      <c r="M62" s="12"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+      <c r="K62" s="14"/>
+      <c r="L62" s="14"/>
+      <c r="M62" s="14"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="H63" s="9"/>
-      <c r="I63" s="12"/>
-      <c r="J63" s="12"/>
-      <c r="K63" s="12"/>
-      <c r="L63" s="12"/>
-      <c r="M63" s="12"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+      <c r="K63" s="14"/>
+      <c r="L63" s="14"/>
+      <c r="M63" s="14"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="H64" s="9"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="12"/>
-      <c r="K64" s="12"/>
-      <c r="L64" s="12"/>
-      <c r="M64" s="12"/>
+      <c r="I64" s="14"/>
+      <c r="J64" s="14"/>
+      <c r="K64" s="14"/>
+      <c r="L64" s="14"/>
+      <c r="M64" s="14"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="H65" s="9"/>
-      <c r="I65" s="12"/>
-      <c r="J65" s="12"/>
-      <c r="K65" s="12"/>
-      <c r="L65" s="12"/>
-      <c r="M65" s="12"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="14"/>
+      <c r="L65" s="14"/>
+      <c r="M65" s="14"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A66" s="13"/>
       <c r="B66" s="13"/>
       <c r="H66" s="9"/>
-      <c r="I66" s="12"/>
-      <c r="J66" s="12"/>
-      <c r="K66" s="12"/>
-      <c r="L66" s="12"/>
-      <c r="M66" s="12"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+      <c r="K66" s="14"/>
+      <c r="L66" s="14"/>
+      <c r="M66" s="14"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="H67" s="9"/>
-      <c r="I67" s="12"/>
-      <c r="J67" s="12"/>
-      <c r="K67" s="12"/>
-      <c r="L67" s="12"/>
-      <c r="M67" s="12"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="14"/>
+      <c r="L67" s="14"/>
+      <c r="M67" s="14"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A68" s="13"/>
       <c r="B68" s="13"/>
       <c r="H68" s="9"/>
-      <c r="I68" s="12"/>
-      <c r="J68" s="12"/>
-      <c r="K68" s="12"/>
-      <c r="L68" s="12"/>
-      <c r="M68" s="12"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+      <c r="K68" s="14"/>
+      <c r="L68" s="14"/>
+      <c r="M68" s="14"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
       <c r="H69" s="9"/>
-      <c r="I69" s="12"/>
-      <c r="J69" s="12"/>
-      <c r="K69" s="12"/>
-      <c r="L69" s="12"/>
-      <c r="M69" s="12"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+      <c r="K69" s="14"/>
+      <c r="L69" s="14"/>
+      <c r="M69" s="14"/>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
       <c r="H70" s="9"/>
-      <c r="I70" s="12"/>
-      <c r="J70" s="12"/>
-      <c r="K70" s="12"/>
-      <c r="L70" s="12"/>
-      <c r="M70" s="12"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="14"/>
+      <c r="K70" s="14"/>
+      <c r="L70" s="14"/>
+      <c r="M70" s="14"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
       <c r="H71" s="9"/>
-      <c r="I71" s="12"/>
-      <c r="J71" s="12"/>
-      <c r="K71" s="12"/>
-      <c r="L71" s="12"/>
-      <c r="M71" s="12"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
+      <c r="K71" s="14"/>
+      <c r="L71" s="14"/>
+      <c r="M71" s="14"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="H72" s="9"/>
-      <c r="I72" s="12"/>
-      <c r="J72" s="12"/>
-      <c r="K72" s="12"/>
-      <c r="L72" s="12"/>
-      <c r="M72" s="12"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+      <c r="K72" s="14"/>
+      <c r="L72" s="14"/>
+      <c r="M72" s="14"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="H73" s="9"/>
-      <c r="I73" s="12"/>
-      <c r="J73" s="12"/>
-      <c r="K73" s="12"/>
-      <c r="L73" s="12"/>
-      <c r="M73" s="12"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="14"/>
+      <c r="L73" s="14"/>
+      <c r="M73" s="14"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="H74" s="9"/>
-      <c r="I74" s="12"/>
-      <c r="J74" s="12"/>
-      <c r="K74" s="12"/>
-      <c r="L74" s="12"/>
-      <c r="M74" s="12"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="14"/>
+      <c r="K74" s="14"/>
+      <c r="L74" s="14"/>
+      <c r="M74" s="14"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="H75" s="9"/>
-      <c r="I75" s="12"/>
-      <c r="J75" s="12"/>
-      <c r="K75" s="12"/>
-      <c r="L75" s="12"/>
-      <c r="M75" s="12"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="14"/>
+      <c r="K75" s="14"/>
+      <c r="L75" s="14"/>
+      <c r="M75" s="14"/>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="H76" s="9"/>
-      <c r="I76" s="12"/>
-      <c r="J76" s="12"/>
-      <c r="K76" s="12"/>
-      <c r="L76" s="12"/>
-      <c r="M76" s="12"/>
+      <c r="I76" s="14"/>
+      <c r="J76" s="14"/>
+      <c r="K76" s="14"/>
+      <c r="L76" s="14"/>
+      <c r="M76" s="14"/>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A77" s="13"/>
       <c r="B77" s="13"/>
       <c r="H77" s="9"/>
-      <c r="I77" s="12"/>
-      <c r="J77" s="12"/>
-      <c r="K77" s="12"/>
-      <c r="L77" s="12"/>
-      <c r="M77" s="12"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="14"/>
+      <c r="K77" s="14"/>
+      <c r="L77" s="14"/>
+      <c r="M77" s="14"/>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A78" s="13"/>
       <c r="B78" s="13"/>
       <c r="H78" s="9"/>
-      <c r="I78" s="12"/>
-      <c r="J78" s="12"/>
-      <c r="K78" s="12"/>
-      <c r="L78" s="12"/>
-      <c r="M78" s="12"/>
+      <c r="I78" s="14"/>
+      <c r="J78" s="14"/>
+      <c r="K78" s="14"/>
+      <c r="L78" s="14"/>
+      <c r="M78" s="14"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A79" s="13"/>
       <c r="B79" s="13"/>
       <c r="H79" s="9"/>
-      <c r="I79" s="12"/>
-      <c r="J79" s="12"/>
-      <c r="K79" s="12"/>
-      <c r="L79" s="12"/>
-      <c r="M79" s="12"/>
+      <c r="I79" s="14"/>
+      <c r="J79" s="14"/>
+      <c r="K79" s="14"/>
+      <c r="L79" s="14"/>
+      <c r="M79" s="14"/>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A80" s="13"/>
       <c r="B80" s="13"/>
       <c r="H80" s="9"/>
-      <c r="I80" s="12"/>
-      <c r="J80" s="12"/>
-      <c r="K80" s="12"/>
-      <c r="L80" s="12"/>
-      <c r="M80" s="12"/>
+      <c r="I80" s="14"/>
+      <c r="J80" s="14"/>
+      <c r="K80" s="14"/>
+      <c r="L80" s="14"/>
+      <c r="M80" s="14"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A81" s="13"/>
       <c r="B81" s="13"/>
       <c r="H81" s="9"/>
-      <c r="I81" s="12"/>
-      <c r="J81" s="12"/>
-      <c r="K81" s="12"/>
-      <c r="L81" s="12"/>
-      <c r="M81" s="12"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="14"/>
+      <c r="K81" s="14"/>
+      <c r="L81" s="14"/>
+      <c r="M81" s="14"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A82" s="13"/>
       <c r="B82" s="13"/>
       <c r="H82" s="9"/>
-      <c r="I82" s="12"/>
-      <c r="J82" s="12"/>
-      <c r="K82" s="12"/>
-      <c r="L82" s="12"/>
-      <c r="M82" s="12"/>
+      <c r="I82" s="14"/>
+      <c r="J82" s="14"/>
+      <c r="K82" s="14"/>
+      <c r="L82" s="14"/>
+      <c r="M82" s="14"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A83" s="13"/>
       <c r="B83" s="13"/>
       <c r="H83" s="9"/>
-      <c r="I83" s="12"/>
-      <c r="J83" s="12"/>
-      <c r="K83" s="12"/>
-      <c r="L83" s="12"/>
-      <c r="M83" s="12"/>
+      <c r="I83" s="14"/>
+      <c r="J83" s="14"/>
+      <c r="K83" s="14"/>
+      <c r="L83" s="14"/>
+      <c r="M83" s="14"/>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A84" s="13"/>
       <c r="B84" s="13"/>
       <c r="H84" s="9"/>
-      <c r="I84" s="12"/>
-      <c r="J84" s="12"/>
-      <c r="K84" s="12"/>
-      <c r="L84" s="12"/>
-      <c r="M84" s="12"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
+      <c r="L84" s="14"/>
+      <c r="M84" s="14"/>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A85" s="13"/>
       <c r="B85" s="13"/>
       <c r="H85" s="9"/>
-      <c r="I85" s="12"/>
-      <c r="J85" s="12"/>
-      <c r="K85" s="12"/>
-      <c r="L85" s="12"/>
-      <c r="M85" s="12"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="14"/>
+      <c r="K85" s="14"/>
+      <c r="L85" s="14"/>
+      <c r="M85" s="14"/>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A86" s="13"/>
       <c r="B86" s="13"/>
       <c r="H86" s="9"/>
-      <c r="I86" s="12"/>
-      <c r="J86" s="12"/>
-      <c r="K86" s="12"/>
-      <c r="L86" s="12"/>
-      <c r="M86" s="12"/>
+      <c r="I86" s="14"/>
+      <c r="J86" s="14"/>
+      <c r="K86" s="14"/>
+      <c r="L86" s="14"/>
+      <c r="M86" s="14"/>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A87" s="13"/>
       <c r="B87" s="13"/>
       <c r="H87" s="9"/>
-      <c r="I87" s="12"/>
-      <c r="J87" s="12"/>
-      <c r="K87" s="12"/>
-      <c r="L87" s="12"/>
-      <c r="M87" s="12"/>
+      <c r="I87" s="14"/>
+      <c r="J87" s="14"/>
+      <c r="K87" s="14"/>
+      <c r="L87" s="14"/>
+      <c r="M87" s="14"/>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A88" s="13"/>
       <c r="B88" s="13"/>
       <c r="H88" s="9"/>
-      <c r="I88" s="12"/>
-      <c r="J88" s="12"/>
-      <c r="K88" s="12"/>
-      <c r="L88" s="12"/>
-      <c r="M88" s="12"/>
+      <c r="I88" s="14"/>
+      <c r="J88" s="14"/>
+      <c r="K88" s="14"/>
+      <c r="L88" s="14"/>
+      <c r="M88" s="14"/>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A89" s="13"/>
       <c r="B89" s="13"/>
       <c r="H89" s="9"/>
-      <c r="I89" s="12"/>
-      <c r="J89" s="12"/>
-      <c r="K89" s="12"/>
-      <c r="L89" s="12"/>
-      <c r="M89" s="12"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="14"/>
+      <c r="K89" s="14"/>
+      <c r="L89" s="14"/>
+      <c r="M89" s="14"/>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A90" s="13"/>
       <c r="B90" s="13"/>
       <c r="H90" s="9"/>
-      <c r="I90" s="12"/>
-      <c r="J90" s="12"/>
-      <c r="K90" s="12"/>
-      <c r="L90" s="12"/>
-      <c r="M90" s="12"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="14"/>
+      <c r="K90" s="14"/>
+      <c r="L90" s="14"/>
+      <c r="M90" s="14"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A91" s="13"/>
       <c r="B91" s="13"/>
       <c r="H91" s="9"/>
-      <c r="I91" s="12"/>
-      <c r="J91" s="12"/>
-      <c r="K91" s="12"/>
-      <c r="L91" s="12"/>
-      <c r="M91" s="12"/>
+      <c r="I91" s="14"/>
+      <c r="J91" s="14"/>
+      <c r="K91" s="14"/>
+      <c r="L91" s="14"/>
+      <c r="M91" s="14"/>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A92" s="13"/>
       <c r="B92" s="13"/>
       <c r="H92" s="9"/>
-      <c r="I92" s="12"/>
-      <c r="J92" s="12"/>
-      <c r="K92" s="12"/>
-      <c r="L92" s="12"/>
-      <c r="M92" s="12"/>
+      <c r="I92" s="14"/>
+      <c r="J92" s="14"/>
+      <c r="K92" s="14"/>
+      <c r="L92" s="14"/>
+      <c r="M92" s="14"/>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A93" s="13"/>
       <c r="B93" s="13"/>
       <c r="H93" s="9"/>
-      <c r="I93" s="12"/>
-      <c r="J93" s="12"/>
-      <c r="K93" s="12"/>
-      <c r="L93" s="12"/>
-      <c r="M93" s="12"/>
+      <c r="I93" s="14"/>
+      <c r="J93" s="14"/>
+      <c r="K93" s="14"/>
+      <c r="L93" s="14"/>
+      <c r="M93" s="14"/>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A94" s="13"/>
       <c r="B94" s="13"/>
       <c r="H94" s="9"/>
-      <c r="I94" s="12"/>
-      <c r="J94" s="12"/>
-      <c r="K94" s="12"/>
-      <c r="L94" s="12"/>
-      <c r="M94" s="12"/>
+      <c r="I94" s="14"/>
+      <c r="J94" s="14"/>
+      <c r="K94" s="14"/>
+      <c r="L94" s="14"/>
+      <c r="M94" s="14"/>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A95" s="13"/>
       <c r="B95" s="13"/>
       <c r="H95" s="9"/>
-      <c r="I95" s="12"/>
-      <c r="J95" s="12"/>
-      <c r="K95" s="12"/>
-      <c r="L95" s="12"/>
-      <c r="M95" s="12"/>
+      <c r="I95" s="14"/>
+      <c r="J95" s="14"/>
+      <c r="K95" s="14"/>
+      <c r="L95" s="14"/>
+      <c r="M95" s="14"/>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A96" s="13"/>
       <c r="B96" s="13"/>
       <c r="H96" s="9"/>
-      <c r="I96" s="12"/>
-      <c r="J96" s="12"/>
-      <c r="K96" s="12"/>
-      <c r="L96" s="12"/>
-      <c r="M96" s="12"/>
+      <c r="I96" s="14"/>
+      <c r="J96" s="14"/>
+      <c r="K96" s="14"/>
+      <c r="L96" s="14"/>
+      <c r="M96" s="14"/>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A97" s="13"/>
       <c r="B97" s="13"/>
       <c r="H97" s="9"/>
-      <c r="I97" s="12"/>
-      <c r="J97" s="12"/>
-      <c r="K97" s="12"/>
-      <c r="L97" s="12"/>
-      <c r="M97" s="12"/>
+      <c r="I97" s="14"/>
+      <c r="J97" s="14"/>
+      <c r="K97" s="14"/>
+      <c r="L97" s="14"/>
+      <c r="M97" s="14"/>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A98" s="13"/>
       <c r="B98" s="13"/>
       <c r="H98" s="9"/>
-      <c r="I98" s="12"/>
-      <c r="J98" s="12"/>
-      <c r="K98" s="12"/>
-      <c r="L98" s="12"/>
-      <c r="M98" s="12"/>
+      <c r="I98" s="14"/>
+      <c r="J98" s="14"/>
+      <c r="K98" s="14"/>
+      <c r="L98" s="14"/>
+      <c r="M98" s="14"/>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A99" s="13"/>
       <c r="B99" s="13"/>
       <c r="H99" s="9"/>
-      <c r="I99" s="12"/>
-      <c r="J99" s="12"/>
-      <c r="K99" s="12"/>
-      <c r="L99" s="12"/>
-      <c r="M99" s="12"/>
+      <c r="I99" s="14"/>
+      <c r="J99" s="14"/>
+      <c r="K99" s="14"/>
+      <c r="L99" s="14"/>
+      <c r="M99" s="14"/>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A100" s="13"/>
       <c r="B100" s="13"/>
       <c r="H100" s="9"/>
-      <c r="I100" s="12"/>
-      <c r="J100" s="12"/>
-      <c r="K100" s="12"/>
-      <c r="L100" s="12"/>
-      <c r="M100" s="12"/>
+      <c r="I100" s="14"/>
+      <c r="J100" s="14"/>
+      <c r="K100" s="14"/>
+      <c r="L100" s="14"/>
+      <c r="M100" s="14"/>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A101" s="13"/>
       <c r="B101" s="13"/>
       <c r="H101" s="9"/>
-      <c r="I101" s="12"/>
-      <c r="J101" s="12"/>
-      <c r="K101" s="12"/>
-      <c r="L101" s="12"/>
-      <c r="M101" s="12"/>
+      <c r="I101" s="14"/>
+      <c r="J101" s="14"/>
+      <c r="K101" s="14"/>
+      <c r="L101" s="14"/>
+      <c r="M101" s="14"/>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A102" s="13"/>
       <c r="B102" s="13"/>
       <c r="H102" s="9"/>
-      <c r="I102" s="12"/>
-      <c r="J102" s="12"/>
-      <c r="K102" s="12"/>
-      <c r="L102" s="12"/>
-      <c r="M102" s="12"/>
+      <c r="I102" s="14"/>
+      <c r="J102" s="14"/>
+      <c r="K102" s="14"/>
+      <c r="L102" s="14"/>
+      <c r="M102" s="14"/>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A103" s="13"/>
       <c r="B103" s="13"/>
       <c r="H103" s="9"/>
-      <c r="I103" s="12"/>
-      <c r="J103" s="12"/>
-      <c r="K103" s="12"/>
-      <c r="L103" s="12"/>
-      <c r="M103" s="12"/>
+      <c r="I103" s="14"/>
+      <c r="J103" s="14"/>
+      <c r="K103" s="14"/>
+      <c r="L103" s="14"/>
+      <c r="M103" s="14"/>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A104" s="13"/>
       <c r="B104" s="13"/>
       <c r="H104" s="9"/>
-      <c r="I104" s="12"/>
-      <c r="J104" s="12"/>
-      <c r="K104" s="12"/>
-      <c r="L104" s="12"/>
-      <c r="M104" s="12"/>
+      <c r="I104" s="14"/>
+      <c r="J104" s="14"/>
+      <c r="K104" s="14"/>
+      <c r="L104" s="14"/>
+      <c r="M104" s="14"/>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A105" s="13"/>
       <c r="B105" s="13"/>
       <c r="H105" s="9"/>
-      <c r="I105" s="12"/>
-      <c r="J105" s="12"/>
-      <c r="K105" s="12"/>
-      <c r="L105" s="12"/>
-      <c r="M105" s="12"/>
+      <c r="I105" s="14"/>
+      <c r="J105" s="14"/>
+      <c r="K105" s="14"/>
+      <c r="L105" s="14"/>
+      <c r="M105" s="14"/>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A106" s="13"/>
       <c r="B106" s="13"/>
       <c r="H106" s="9"/>
-      <c r="I106" s="12"/>
-      <c r="J106" s="12"/>
-      <c r="K106" s="12"/>
-      <c r="L106" s="12"/>
-      <c r="M106" s="12"/>
+      <c r="I106" s="14"/>
+      <c r="J106" s="14"/>
+      <c r="K106" s="14"/>
+      <c r="L106" s="14"/>
+      <c r="M106" s="14"/>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A107" s="13"/>
       <c r="B107" s="13"/>
       <c r="H107" s="9"/>
-      <c r="I107" s="12"/>
-      <c r="J107" s="12"/>
-      <c r="K107" s="12"/>
-      <c r="L107" s="12"/>
-      <c r="M107" s="12"/>
+      <c r="I107" s="14"/>
+      <c r="J107" s="14"/>
+      <c r="K107" s="14"/>
+      <c r="L107" s="14"/>
+      <c r="M107" s="14"/>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A108" s="13"/>
       <c r="B108" s="13"/>
       <c r="H108" s="9"/>
-      <c r="I108" s="12"/>
-      <c r="J108" s="12"/>
-      <c r="K108" s="12"/>
-      <c r="L108" s="12"/>
-      <c r="M108" s="12"/>
+      <c r="I108" s="14"/>
+      <c r="J108" s="14"/>
+      <c r="K108" s="14"/>
+      <c r="L108" s="14"/>
+      <c r="M108" s="14"/>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A109" s="13"/>
       <c r="B109" s="13"/>
       <c r="H109" s="9"/>
-      <c r="I109" s="12"/>
-      <c r="J109" s="12"/>
-      <c r="K109" s="12"/>
-      <c r="L109" s="12"/>
-      <c r="M109" s="12"/>
+      <c r="I109" s="14"/>
+      <c r="J109" s="14"/>
+      <c r="K109" s="14"/>
+      <c r="L109" s="14"/>
+      <c r="M109" s="14"/>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A110" s="13"/>
       <c r="B110" s="13"/>
       <c r="H110" s="9"/>
-      <c r="I110" s="12"/>
-      <c r="J110" s="12"/>
-      <c r="K110" s="12"/>
-      <c r="L110" s="12"/>
-      <c r="M110" s="12"/>
+      <c r="I110" s="14"/>
+      <c r="J110" s="14"/>
+      <c r="K110" s="14"/>
+      <c r="L110" s="14"/>
+      <c r="M110" s="14"/>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A111" s="13"/>
       <c r="B111" s="13"/>
       <c r="H111" s="9"/>
-      <c r="I111" s="9"/>
-      <c r="J111" s="9"/>
-      <c r="K111" s="9"/>
-      <c r="L111" s="9"/>
-      <c r="M111" s="9"/>
+      <c r="I111" s="14"/>
+      <c r="J111" s="14"/>
+      <c r="K111" s="14"/>
+      <c r="L111" s="14"/>
+      <c r="M111" s="14"/>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A112" s="13"/>
@@ -3312,6 +3321,12 @@
     <row r="117" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A117" s="13"/>
       <c r="B117" s="13"/>
+      <c r="H117" s="9"/>
+      <c r="I117" s="9"/>
+      <c r="J117" s="9"/>
+      <c r="K117" s="9"/>
+      <c r="L117" s="9"/>
+      <c r="M117" s="9"/>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.6">
       <c r="A118" s="13"/>
@@ -3408,7 +3423,6 @@
     <row r="141" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A141" s="13"/>
       <c r="B141" s="13"/>
-      <c r="D141" s="5"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A142" s="13"/>
@@ -3478,6 +3492,7 @@
     <row r="155" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A155" s="13"/>
       <c r="B155" s="13"/>
+      <c r="D155" s="5"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A156" s="13"/>
@@ -3498,7 +3513,6 @@
     <row r="160" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A160" s="13"/>
       <c r="B160" s="13"/>
-      <c r="D160" s="5"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A161" s="13"/>
@@ -3813,11 +3827,11 @@
     <row r="223" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A223" s="13"/>
       <c r="B223" s="13"/>
+      <c r="D223" s="5"/>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A224" s="13"/>
       <c r="B224" s="13"/>
-      <c r="D224" s="5"/>
     </row>
     <row r="225" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A225" s="13"/>
@@ -3833,876 +3847,876 @@
       <c r="A227" s="13"/>
       <c r="B227" s="13"/>
       <c r="D227" s="5"/>
-      <c r="I227" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J227" s="12"/>
-      <c r="K227" s="12"/>
-      <c r="L227" s="12"/>
-      <c r="M227" s="12"/>
-      <c r="N227" s="12"/>
-      <c r="O227" s="12"/>
     </row>
     <row r="228" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A228" s="13"/>
       <c r="B228" s="13"/>
       <c r="D228" s="5"/>
-      <c r="I228" s="12"/>
-      <c r="J228" s="12"/>
-      <c r="K228" s="12"/>
-      <c r="L228" s="12"/>
-      <c r="M228" s="12"/>
-      <c r="N228" s="12"/>
-      <c r="O228" s="12"/>
+      <c r="I228" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J228" s="14"/>
+      <c r="K228" s="14"/>
+      <c r="L228" s="14"/>
+      <c r="M228" s="14"/>
+      <c r="N228" s="14"/>
+      <c r="O228" s="14"/>
     </row>
     <row r="229" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A229" s="13"/>
       <c r="B229" s="13"/>
       <c r="D229" s="5"/>
-      <c r="I229" s="12"/>
-      <c r="J229" s="12"/>
-      <c r="K229" s="12"/>
-      <c r="L229" s="12"/>
-      <c r="M229" s="12"/>
-      <c r="N229" s="12"/>
-      <c r="O229" s="12"/>
+      <c r="I229" s="14"/>
+      <c r="J229" s="14"/>
+      <c r="K229" s="14"/>
+      <c r="L229" s="14"/>
+      <c r="M229" s="14"/>
+      <c r="N229" s="14"/>
+      <c r="O229" s="14"/>
     </row>
     <row r="230" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A230" s="13"/>
       <c r="B230" s="13"/>
       <c r="D230" s="5"/>
-      <c r="I230" s="12"/>
-      <c r="J230" s="12"/>
-      <c r="K230" s="12"/>
-      <c r="L230" s="12"/>
-      <c r="M230" s="12"/>
-      <c r="N230" s="12"/>
-      <c r="O230" s="12"/>
+      <c r="I230" s="14"/>
+      <c r="J230" s="14"/>
+      <c r="K230" s="14"/>
+      <c r="L230" s="14"/>
+      <c r="M230" s="14"/>
+      <c r="N230" s="14"/>
+      <c r="O230" s="14"/>
     </row>
     <row r="231" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A231" s="13"/>
       <c r="B231" s="13"/>
       <c r="D231" s="5"/>
-      <c r="I231" s="12"/>
-      <c r="J231" s="12"/>
-      <c r="K231" s="12"/>
-      <c r="L231" s="12"/>
-      <c r="M231" s="12"/>
-      <c r="N231" s="12"/>
-      <c r="O231" s="12"/>
+      <c r="I231" s="14"/>
+      <c r="J231" s="14"/>
+      <c r="K231" s="14"/>
+      <c r="L231" s="14"/>
+      <c r="M231" s="14"/>
+      <c r="N231" s="14"/>
+      <c r="O231" s="14"/>
     </row>
     <row r="232" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A232" s="13"/>
       <c r="B232" s="13"/>
       <c r="D232" s="5"/>
-      <c r="I232" s="12"/>
-      <c r="J232" s="12"/>
-      <c r="K232" s="12"/>
-      <c r="L232" s="12"/>
-      <c r="M232" s="12"/>
-      <c r="N232" s="12"/>
-      <c r="O232" s="12"/>
+      <c r="I232" s="14"/>
+      <c r="J232" s="14"/>
+      <c r="K232" s="14"/>
+      <c r="L232" s="14"/>
+      <c r="M232" s="14"/>
+      <c r="N232" s="14"/>
+      <c r="O232" s="14"/>
     </row>
     <row r="233" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A233" s="13"/>
       <c r="B233" s="13"/>
       <c r="D233" s="5"/>
-      <c r="I233" s="12"/>
-      <c r="J233" s="12"/>
-      <c r="K233" s="12"/>
-      <c r="L233" s="12"/>
-      <c r="M233" s="12"/>
-      <c r="N233" s="12"/>
-      <c r="O233" s="12"/>
+      <c r="I233" s="14"/>
+      <c r="J233" s="14"/>
+      <c r="K233" s="14"/>
+      <c r="L233" s="14"/>
+      <c r="M233" s="14"/>
+      <c r="N233" s="14"/>
+      <c r="O233" s="14"/>
     </row>
     <row r="234" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A234" s="13"/>
       <c r="B234" s="13"/>
       <c r="D234" s="5"/>
-      <c r="I234" s="12"/>
-      <c r="J234" s="12"/>
-      <c r="K234" s="12"/>
-      <c r="L234" s="12"/>
-      <c r="M234" s="12"/>
-      <c r="N234" s="12"/>
-      <c r="O234" s="12"/>
+      <c r="I234" s="14"/>
+      <c r="J234" s="14"/>
+      <c r="K234" s="14"/>
+      <c r="L234" s="14"/>
+      <c r="M234" s="14"/>
+      <c r="N234" s="14"/>
+      <c r="O234" s="14"/>
     </row>
     <row r="235" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A235" s="13"/>
       <c r="B235" s="13"/>
       <c r="D235" s="5"/>
-      <c r="I235" s="12"/>
-      <c r="J235" s="12"/>
-      <c r="K235" s="12"/>
-      <c r="L235" s="12"/>
-      <c r="M235" s="12"/>
-      <c r="N235" s="12"/>
-      <c r="O235" s="12"/>
+      <c r="I235" s="14"/>
+      <c r="J235" s="14"/>
+      <c r="K235" s="14"/>
+      <c r="L235" s="14"/>
+      <c r="M235" s="14"/>
+      <c r="N235" s="14"/>
+      <c r="O235" s="14"/>
     </row>
     <row r="236" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A236" s="13"/>
       <c r="B236" s="13"/>
       <c r="D236" s="5"/>
-      <c r="I236" s="12"/>
-      <c r="J236" s="12"/>
-      <c r="K236" s="12"/>
-      <c r="L236" s="12"/>
-      <c r="M236" s="12"/>
-      <c r="N236" s="12"/>
-      <c r="O236" s="12"/>
+      <c r="I236" s="14"/>
+      <c r="J236" s="14"/>
+      <c r="K236" s="14"/>
+      <c r="L236" s="14"/>
+      <c r="M236" s="14"/>
+      <c r="N236" s="14"/>
+      <c r="O236" s="14"/>
     </row>
     <row r="237" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A237" s="13"/>
       <c r="B237" s="13"/>
       <c r="D237" s="5"/>
-      <c r="I237" s="12"/>
-      <c r="J237" s="12"/>
-      <c r="K237" s="12"/>
-      <c r="L237" s="12"/>
-      <c r="M237" s="12"/>
-      <c r="N237" s="12"/>
-      <c r="O237" s="12"/>
+      <c r="I237" s="14"/>
+      <c r="J237" s="14"/>
+      <c r="K237" s="14"/>
+      <c r="L237" s="14"/>
+      <c r="M237" s="14"/>
+      <c r="N237" s="14"/>
+      <c r="O237" s="14"/>
     </row>
     <row r="238" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A238" s="13"/>
       <c r="B238" s="13"/>
       <c r="D238" s="5"/>
-      <c r="I238" s="12"/>
-      <c r="J238" s="12"/>
-      <c r="K238" s="12"/>
-      <c r="L238" s="12"/>
-      <c r="M238" s="12"/>
-      <c r="N238" s="12"/>
-      <c r="O238" s="12"/>
+      <c r="I238" s="14"/>
+      <c r="J238" s="14"/>
+      <c r="K238" s="14"/>
+      <c r="L238" s="14"/>
+      <c r="M238" s="14"/>
+      <c r="N238" s="14"/>
+      <c r="O238" s="14"/>
     </row>
     <row r="239" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A239" s="13"/>
       <c r="B239" s="13"/>
       <c r="D239" s="5"/>
-      <c r="I239" s="12"/>
-      <c r="J239" s="12"/>
-      <c r="K239" s="12"/>
-      <c r="L239" s="12"/>
-      <c r="M239" s="12"/>
-      <c r="N239" s="12"/>
-      <c r="O239" s="12"/>
+      <c r="I239" s="14"/>
+      <c r="J239" s="14"/>
+      <c r="K239" s="14"/>
+      <c r="L239" s="14"/>
+      <c r="M239" s="14"/>
+      <c r="N239" s="14"/>
+      <c r="O239" s="14"/>
     </row>
     <row r="240" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A240" s="13"/>
       <c r="B240" s="13"/>
       <c r="D240" s="5"/>
-      <c r="I240" s="12"/>
-      <c r="J240" s="12"/>
-      <c r="K240" s="12"/>
-      <c r="L240" s="12"/>
-      <c r="M240" s="12"/>
-      <c r="N240" s="12"/>
-      <c r="O240" s="12"/>
+      <c r="I240" s="14"/>
+      <c r="J240" s="14"/>
+      <c r="K240" s="14"/>
+      <c r="L240" s="14"/>
+      <c r="M240" s="14"/>
+      <c r="N240" s="14"/>
+      <c r="O240" s="14"/>
     </row>
     <row r="241" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A241" s="13"/>
       <c r="B241" s="13"/>
       <c r="D241" s="5"/>
-      <c r="I241" s="12"/>
-      <c r="J241" s="12"/>
-      <c r="K241" s="12"/>
-      <c r="L241" s="12"/>
-      <c r="M241" s="12"/>
-      <c r="N241" s="12"/>
-      <c r="O241" s="12"/>
+      <c r="I241" s="14"/>
+      <c r="J241" s="14"/>
+      <c r="K241" s="14"/>
+      <c r="L241" s="14"/>
+      <c r="M241" s="14"/>
+      <c r="N241" s="14"/>
+      <c r="O241" s="14"/>
     </row>
     <row r="242" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A242" s="13"/>
       <c r="B242" s="13"/>
       <c r="D242" s="5"/>
-      <c r="I242" s="12"/>
-      <c r="J242" s="12"/>
-      <c r="K242" s="12"/>
-      <c r="L242" s="12"/>
-      <c r="M242" s="12"/>
-      <c r="N242" s="12"/>
-      <c r="O242" s="12"/>
+      <c r="I242" s="14"/>
+      <c r="J242" s="14"/>
+      <c r="K242" s="14"/>
+      <c r="L242" s="14"/>
+      <c r="M242" s="14"/>
+      <c r="N242" s="14"/>
+      <c r="O242" s="14"/>
     </row>
     <row r="243" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A243" s="13"/>
       <c r="B243" s="13"/>
       <c r="D243" s="5"/>
-      <c r="I243" s="12"/>
-      <c r="J243" s="12"/>
-      <c r="K243" s="12"/>
-      <c r="L243" s="12"/>
-      <c r="M243" s="12"/>
-      <c r="N243" s="12"/>
-      <c r="O243" s="12"/>
+      <c r="I243" s="14"/>
+      <c r="J243" s="14"/>
+      <c r="K243" s="14"/>
+      <c r="L243" s="14"/>
+      <c r="M243" s="14"/>
+      <c r="N243" s="14"/>
+      <c r="O243" s="14"/>
     </row>
     <row r="244" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A244" s="13"/>
       <c r="B244" s="13"/>
       <c r="D244" s="5"/>
-      <c r="I244" s="12"/>
-      <c r="J244" s="12"/>
-      <c r="K244" s="12"/>
-      <c r="L244" s="12"/>
-      <c r="M244" s="12"/>
-      <c r="N244" s="12"/>
-      <c r="O244" s="12"/>
+      <c r="I244" s="14"/>
+      <c r="J244" s="14"/>
+      <c r="K244" s="14"/>
+      <c r="L244" s="14"/>
+      <c r="M244" s="14"/>
+      <c r="N244" s="14"/>
+      <c r="O244" s="14"/>
     </row>
     <row r="245" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A245" s="13"/>
       <c r="B245" s="13"/>
       <c r="D245" s="5"/>
-      <c r="I245" s="12"/>
-      <c r="J245" s="12"/>
-      <c r="K245" s="12"/>
-      <c r="L245" s="12"/>
-      <c r="M245" s="12"/>
-      <c r="N245" s="12"/>
-      <c r="O245" s="12"/>
+      <c r="I245" s="14"/>
+      <c r="J245" s="14"/>
+      <c r="K245" s="14"/>
+      <c r="L245" s="14"/>
+      <c r="M245" s="14"/>
+      <c r="N245" s="14"/>
+      <c r="O245" s="14"/>
     </row>
     <row r="246" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A246" s="13"/>
       <c r="B246" s="13"/>
       <c r="D246" s="5"/>
-      <c r="I246" s="12"/>
-      <c r="J246" s="12"/>
-      <c r="K246" s="12"/>
-      <c r="L246" s="12"/>
-      <c r="M246" s="12"/>
-      <c r="N246" s="12"/>
-      <c r="O246" s="12"/>
+      <c r="I246" s="14"/>
+      <c r="J246" s="14"/>
+      <c r="K246" s="14"/>
+      <c r="L246" s="14"/>
+      <c r="M246" s="14"/>
+      <c r="N246" s="14"/>
+      <c r="O246" s="14"/>
     </row>
     <row r="247" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A247" s="13"/>
       <c r="B247" s="13"/>
       <c r="D247" s="5"/>
-      <c r="I247" s="12"/>
-      <c r="J247" s="12"/>
-      <c r="K247" s="12"/>
-      <c r="L247" s="12"/>
-      <c r="M247" s="12"/>
-      <c r="N247" s="12"/>
-      <c r="O247" s="12"/>
+      <c r="I247" s="14"/>
+      <c r="J247" s="14"/>
+      <c r="K247" s="14"/>
+      <c r="L247" s="14"/>
+      <c r="M247" s="14"/>
+      <c r="N247" s="14"/>
+      <c r="O247" s="14"/>
     </row>
     <row r="248" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A248" s="13"/>
       <c r="B248" s="13"/>
       <c r="D248" s="5"/>
-      <c r="I248" s="12"/>
-      <c r="J248" s="12"/>
-      <c r="K248" s="12"/>
-      <c r="L248" s="12"/>
-      <c r="M248" s="12"/>
-      <c r="N248" s="12"/>
-      <c r="O248" s="12"/>
+      <c r="I248" s="14"/>
+      <c r="J248" s="14"/>
+      <c r="K248" s="14"/>
+      <c r="L248" s="14"/>
+      <c r="M248" s="14"/>
+      <c r="N248" s="14"/>
+      <c r="O248" s="14"/>
     </row>
     <row r="249" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A249" s="13"/>
       <c r="B249" s="13"/>
       <c r="D249" s="5"/>
-      <c r="I249" s="12"/>
-      <c r="J249" s="12"/>
-      <c r="K249" s="12"/>
-      <c r="L249" s="12"/>
-      <c r="M249" s="12"/>
-      <c r="N249" s="12"/>
-      <c r="O249" s="12"/>
+      <c r="I249" s="14"/>
+      <c r="J249" s="14"/>
+      <c r="K249" s="14"/>
+      <c r="L249" s="14"/>
+      <c r="M249" s="14"/>
+      <c r="N249" s="14"/>
+      <c r="O249" s="14"/>
     </row>
     <row r="250" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A250" s="13"/>
       <c r="B250" s="13"/>
       <c r="D250" s="5"/>
-      <c r="I250" s="12"/>
-      <c r="J250" s="12"/>
-      <c r="K250" s="12"/>
-      <c r="L250" s="12"/>
-      <c r="M250" s="12"/>
-      <c r="N250" s="12"/>
-      <c r="O250" s="12"/>
+      <c r="I250" s="14"/>
+      <c r="J250" s="14"/>
+      <c r="K250" s="14"/>
+      <c r="L250" s="14"/>
+      <c r="M250" s="14"/>
+      <c r="N250" s="14"/>
+      <c r="O250" s="14"/>
     </row>
     <row r="251" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A251" s="13"/>
       <c r="B251" s="13"/>
       <c r="D251" s="5"/>
-      <c r="I251" s="12"/>
-      <c r="J251" s="12"/>
-      <c r="K251" s="12"/>
-      <c r="L251" s="12"/>
-      <c r="M251" s="12"/>
-      <c r="N251" s="12"/>
-      <c r="O251" s="12"/>
+      <c r="I251" s="14"/>
+      <c r="J251" s="14"/>
+      <c r="K251" s="14"/>
+      <c r="L251" s="14"/>
+      <c r="M251" s="14"/>
+      <c r="N251" s="14"/>
+      <c r="O251" s="14"/>
     </row>
     <row r="252" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A252" s="13"/>
       <c r="B252" s="13"/>
       <c r="D252" s="5"/>
-      <c r="I252" s="12"/>
-      <c r="J252" s="12"/>
-      <c r="K252" s="12"/>
-      <c r="L252" s="12"/>
-      <c r="M252" s="12"/>
-      <c r="N252" s="12"/>
-      <c r="O252" s="12"/>
+      <c r="I252" s="14"/>
+      <c r="J252" s="14"/>
+      <c r="K252" s="14"/>
+      <c r="L252" s="14"/>
+      <c r="M252" s="14"/>
+      <c r="N252" s="14"/>
+      <c r="O252" s="14"/>
     </row>
     <row r="253" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A253" s="13"/>
       <c r="B253" s="13"/>
       <c r="D253" s="5"/>
-      <c r="I253" s="12"/>
-      <c r="J253" s="12"/>
-      <c r="K253" s="12"/>
-      <c r="L253" s="12"/>
-      <c r="M253" s="12"/>
-      <c r="N253" s="12"/>
-      <c r="O253" s="12"/>
+      <c r="I253" s="14"/>
+      <c r="J253" s="14"/>
+      <c r="K253" s="14"/>
+      <c r="L253" s="14"/>
+      <c r="M253" s="14"/>
+      <c r="N253" s="14"/>
+      <c r="O253" s="14"/>
     </row>
     <row r="254" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A254" s="13"/>
       <c r="B254" s="13"/>
       <c r="D254" s="5"/>
-      <c r="I254" s="12"/>
-      <c r="J254" s="12"/>
-      <c r="K254" s="12"/>
-      <c r="L254" s="12"/>
-      <c r="M254" s="12"/>
-      <c r="N254" s="12"/>
-      <c r="O254" s="12"/>
+      <c r="I254" s="14"/>
+      <c r="J254" s="14"/>
+      <c r="K254" s="14"/>
+      <c r="L254" s="14"/>
+      <c r="M254" s="14"/>
+      <c r="N254" s="14"/>
+      <c r="O254" s="14"/>
     </row>
     <row r="255" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A255" s="13"/>
       <c r="B255" s="13"/>
       <c r="D255" s="5"/>
-      <c r="I255" s="12"/>
-      <c r="J255" s="12"/>
-      <c r="K255" s="12"/>
-      <c r="L255" s="12"/>
-      <c r="M255" s="12"/>
-      <c r="N255" s="12"/>
-      <c r="O255" s="12"/>
+      <c r="I255" s="14"/>
+      <c r="J255" s="14"/>
+      <c r="K255" s="14"/>
+      <c r="L255" s="14"/>
+      <c r="M255" s="14"/>
+      <c r="N255" s="14"/>
+      <c r="O255" s="14"/>
     </row>
     <row r="256" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A256" s="13"/>
       <c r="B256" s="13"/>
       <c r="D256" s="5"/>
-      <c r="I256" s="12"/>
-      <c r="J256" s="12"/>
-      <c r="K256" s="12"/>
-      <c r="L256" s="12"/>
-      <c r="M256" s="12"/>
-      <c r="N256" s="12"/>
-      <c r="O256" s="12"/>
+      <c r="I256" s="14"/>
+      <c r="J256" s="14"/>
+      <c r="K256" s="14"/>
+      <c r="L256" s="14"/>
+      <c r="M256" s="14"/>
+      <c r="N256" s="14"/>
+      <c r="O256" s="14"/>
     </row>
     <row r="257" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A257" s="13"/>
       <c r="B257" s="13"/>
       <c r="D257" s="5"/>
-      <c r="I257" s="12"/>
-      <c r="J257" s="12"/>
-      <c r="K257" s="12"/>
-      <c r="L257" s="12"/>
-      <c r="M257" s="12"/>
-      <c r="N257" s="12"/>
-      <c r="O257" s="12"/>
+      <c r="I257" s="14"/>
+      <c r="J257" s="14"/>
+      <c r="K257" s="14"/>
+      <c r="L257" s="14"/>
+      <c r="M257" s="14"/>
+      <c r="N257" s="14"/>
+      <c r="O257" s="14"/>
     </row>
     <row r="258" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A258" s="13"/>
       <c r="B258" s="13"/>
       <c r="D258" s="5"/>
-      <c r="I258" s="12"/>
-      <c r="J258" s="12"/>
-      <c r="K258" s="12"/>
-      <c r="L258" s="12"/>
-      <c r="M258" s="12"/>
-      <c r="N258" s="12"/>
-      <c r="O258" s="12"/>
+      <c r="I258" s="14"/>
+      <c r="J258" s="14"/>
+      <c r="K258" s="14"/>
+      <c r="L258" s="14"/>
+      <c r="M258" s="14"/>
+      <c r="N258" s="14"/>
+      <c r="O258" s="14"/>
     </row>
     <row r="259" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A259" s="13"/>
       <c r="B259" s="13"/>
       <c r="D259" s="5"/>
-      <c r="I259" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="J259" s="12"/>
-      <c r="K259" s="12"/>
-      <c r="L259" s="12"/>
-      <c r="M259" s="12"/>
-      <c r="N259" s="12"/>
-      <c r="O259" s="12"/>
+      <c r="I259" s="14"/>
+      <c r="J259" s="14"/>
+      <c r="K259" s="14"/>
+      <c r="L259" s="14"/>
+      <c r="M259" s="14"/>
+      <c r="N259" s="14"/>
+      <c r="O259" s="14"/>
     </row>
     <row r="260" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A260" s="13"/>
       <c r="B260" s="13"/>
       <c r="D260" s="5"/>
-      <c r="I260" s="12"/>
-      <c r="J260" s="12"/>
-      <c r="K260" s="12"/>
-      <c r="L260" s="12"/>
-      <c r="M260" s="12"/>
-      <c r="N260" s="12"/>
-      <c r="O260" s="12"/>
+      <c r="I260" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J260" s="14"/>
+      <c r="K260" s="14"/>
+      <c r="L260" s="14"/>
+      <c r="M260" s="14"/>
+      <c r="N260" s="14"/>
+      <c r="O260" s="14"/>
     </row>
     <row r="261" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A261" s="13"/>
       <c r="B261" s="13"/>
       <c r="D261" s="5"/>
-      <c r="I261" s="12"/>
-      <c r="J261" s="12"/>
-      <c r="K261" s="12"/>
-      <c r="L261" s="12"/>
-      <c r="M261" s="12"/>
-      <c r="N261" s="12"/>
-      <c r="O261" s="12"/>
+      <c r="I261" s="14"/>
+      <c r="J261" s="14"/>
+      <c r="K261" s="14"/>
+      <c r="L261" s="14"/>
+      <c r="M261" s="14"/>
+      <c r="N261" s="14"/>
+      <c r="O261" s="14"/>
     </row>
     <row r="262" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A262" s="13"/>
       <c r="B262" s="13"/>
       <c r="D262" s="5"/>
-      <c r="I262" s="12"/>
-      <c r="J262" s="12"/>
-      <c r="K262" s="12"/>
-      <c r="L262" s="12"/>
-      <c r="M262" s="12"/>
-      <c r="N262" s="12"/>
-      <c r="O262" s="12"/>
+      <c r="I262" s="14"/>
+      <c r="J262" s="14"/>
+      <c r="K262" s="14"/>
+      <c r="L262" s="14"/>
+      <c r="M262" s="14"/>
+      <c r="N262" s="14"/>
+      <c r="O262" s="14"/>
     </row>
     <row r="263" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A263" s="13"/>
       <c r="B263" s="13"/>
       <c r="D263" s="5"/>
-      <c r="I263" s="12"/>
-      <c r="J263" s="12"/>
-      <c r="K263" s="12"/>
-      <c r="L263" s="12"/>
-      <c r="M263" s="12"/>
-      <c r="N263" s="12"/>
-      <c r="O263" s="12"/>
+      <c r="I263" s="14"/>
+      <c r="J263" s="14"/>
+      <c r="K263" s="14"/>
+      <c r="L263" s="14"/>
+      <c r="M263" s="14"/>
+      <c r="N263" s="14"/>
+      <c r="O263" s="14"/>
     </row>
     <row r="264" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A264" s="13"/>
       <c r="B264" s="13"/>
       <c r="D264" s="5"/>
-      <c r="I264" s="12"/>
-      <c r="J264" s="12"/>
-      <c r="K264" s="12"/>
-      <c r="L264" s="12"/>
-      <c r="M264" s="12"/>
-      <c r="N264" s="12"/>
-      <c r="O264" s="12"/>
+      <c r="I264" s="14"/>
+      <c r="J264" s="14"/>
+      <c r="K264" s="14"/>
+      <c r="L264" s="14"/>
+      <c r="M264" s="14"/>
+      <c r="N264" s="14"/>
+      <c r="O264" s="14"/>
     </row>
     <row r="265" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A265" s="13"/>
       <c r="B265" s="13"/>
       <c r="D265" s="5"/>
-      <c r="I265" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J265" s="12"/>
-      <c r="K265" s="12"/>
-      <c r="L265" s="12"/>
-      <c r="M265" s="12"/>
-      <c r="N265" s="12"/>
-      <c r="O265" s="12"/>
+      <c r="I265" s="14"/>
+      <c r="J265" s="14"/>
+      <c r="K265" s="14"/>
+      <c r="L265" s="14"/>
+      <c r="M265" s="14"/>
+      <c r="N265" s="14"/>
+      <c r="O265" s="14"/>
     </row>
     <row r="266" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A266" s="13"/>
       <c r="B266" s="13"/>
       <c r="D266" s="5"/>
-      <c r="I266" s="12"/>
-      <c r="J266" s="12"/>
-      <c r="K266" s="12"/>
-      <c r="L266" s="12"/>
-      <c r="M266" s="12"/>
-      <c r="N266" s="12"/>
-      <c r="O266" s="12"/>
+      <c r="I266" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J266" s="14"/>
+      <c r="K266" s="14"/>
+      <c r="L266" s="14"/>
+      <c r="M266" s="14"/>
+      <c r="N266" s="14"/>
+      <c r="O266" s="14"/>
     </row>
     <row r="267" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A267" s="13"/>
       <c r="B267" s="13"/>
       <c r="D267" s="5"/>
-      <c r="I267" s="12"/>
-      <c r="J267" s="12"/>
-      <c r="K267" s="12"/>
-      <c r="L267" s="12"/>
-      <c r="M267" s="12"/>
-      <c r="N267" s="12"/>
-      <c r="O267" s="12"/>
+      <c r="I267" s="14"/>
+      <c r="J267" s="14"/>
+      <c r="K267" s="14"/>
+      <c r="L267" s="14"/>
+      <c r="M267" s="14"/>
+      <c r="N267" s="14"/>
+      <c r="O267" s="14"/>
     </row>
     <row r="268" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A268" s="13"/>
       <c r="B268" s="13"/>
       <c r="D268" s="5"/>
-      <c r="I268" s="12"/>
-      <c r="J268" s="12"/>
-      <c r="K268" s="12"/>
-      <c r="L268" s="12"/>
-      <c r="M268" s="12"/>
-      <c r="N268" s="12"/>
-      <c r="O268" s="12"/>
+      <c r="I268" s="14"/>
+      <c r="J268" s="14"/>
+      <c r="K268" s="14"/>
+      <c r="L268" s="14"/>
+      <c r="M268" s="14"/>
+      <c r="N268" s="14"/>
+      <c r="O268" s="14"/>
     </row>
     <row r="269" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A269" s="13"/>
       <c r="B269" s="13"/>
       <c r="D269" s="5"/>
-      <c r="I269" s="12"/>
-      <c r="J269" s="12"/>
-      <c r="K269" s="12"/>
-      <c r="L269" s="12"/>
-      <c r="M269" s="12"/>
-      <c r="N269" s="12"/>
-      <c r="O269" s="12"/>
+      <c r="I269" s="14"/>
+      <c r="J269" s="14"/>
+      <c r="K269" s="14"/>
+      <c r="L269" s="14"/>
+      <c r="M269" s="14"/>
+      <c r="N269" s="14"/>
+      <c r="O269" s="14"/>
     </row>
     <row r="270" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A270" s="13"/>
       <c r="B270" s="13"/>
       <c r="D270" s="5"/>
-      <c r="I270" s="12"/>
-      <c r="J270" s="12"/>
-      <c r="K270" s="12"/>
-      <c r="L270" s="12"/>
-      <c r="M270" s="12"/>
-      <c r="N270" s="12"/>
-      <c r="O270" s="12"/>
+      <c r="I270" s="14"/>
+      <c r="J270" s="14"/>
+      <c r="K270" s="14"/>
+      <c r="L270" s="14"/>
+      <c r="M270" s="14"/>
+      <c r="N270" s="14"/>
+      <c r="O270" s="14"/>
     </row>
     <row r="271" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A271" s="13"/>
       <c r="B271" s="13"/>
       <c r="D271" s="5"/>
-      <c r="I271" s="12"/>
-      <c r="J271" s="12"/>
-      <c r="K271" s="12"/>
-      <c r="L271" s="12"/>
-      <c r="M271" s="12"/>
-      <c r="N271" s="12"/>
-      <c r="O271" s="12"/>
+      <c r="I271" s="14"/>
+      <c r="J271" s="14"/>
+      <c r="K271" s="14"/>
+      <c r="L271" s="14"/>
+      <c r="M271" s="14"/>
+      <c r="N271" s="14"/>
+      <c r="O271" s="14"/>
     </row>
     <row r="272" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A272" s="13"/>
       <c r="B272" s="13"/>
       <c r="D272" s="5"/>
-      <c r="I272" s="12"/>
-      <c r="J272" s="12"/>
-      <c r="K272" s="12"/>
-      <c r="L272" s="12"/>
-      <c r="M272" s="12"/>
-      <c r="N272" s="12"/>
-      <c r="O272" s="12"/>
+      <c r="I272" s="14"/>
+      <c r="J272" s="14"/>
+      <c r="K272" s="14"/>
+      <c r="L272" s="14"/>
+      <c r="M272" s="14"/>
+      <c r="N272" s="14"/>
+      <c r="O272" s="14"/>
     </row>
     <row r="273" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A273" s="13"/>
       <c r="B273" s="13"/>
       <c r="D273" s="5"/>
-      <c r="I273" s="12"/>
-      <c r="J273" s="12"/>
-      <c r="K273" s="12"/>
-      <c r="L273" s="12"/>
-      <c r="M273" s="12"/>
-      <c r="N273" s="12"/>
-      <c r="O273" s="12"/>
+      <c r="I273" s="14"/>
+      <c r="J273" s="14"/>
+      <c r="K273" s="14"/>
+      <c r="L273" s="14"/>
+      <c r="M273" s="14"/>
+      <c r="N273" s="14"/>
+      <c r="O273" s="14"/>
     </row>
     <row r="274" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A274" s="13"/>
       <c r="B274" s="13"/>
       <c r="D274" s="5"/>
-      <c r="I274" s="12"/>
-      <c r="J274" s="12"/>
-      <c r="K274" s="12"/>
-      <c r="L274" s="12"/>
-      <c r="M274" s="12"/>
-      <c r="N274" s="12"/>
-      <c r="O274" s="12"/>
+      <c r="I274" s="14"/>
+      <c r="J274" s="14"/>
+      <c r="K274" s="14"/>
+      <c r="L274" s="14"/>
+      <c r="M274" s="14"/>
+      <c r="N274" s="14"/>
+      <c r="O274" s="14"/>
     </row>
     <row r="275" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A275" s="13"/>
       <c r="B275" s="13"/>
       <c r="D275" s="5"/>
-      <c r="I275" s="12"/>
-      <c r="J275" s="12"/>
-      <c r="K275" s="12"/>
-      <c r="L275" s="12"/>
-      <c r="M275" s="12"/>
-      <c r="N275" s="12"/>
-      <c r="O275" s="12"/>
+      <c r="I275" s="14"/>
+      <c r="J275" s="14"/>
+      <c r="K275" s="14"/>
+      <c r="L275" s="14"/>
+      <c r="M275" s="14"/>
+      <c r="N275" s="14"/>
+      <c r="O275" s="14"/>
     </row>
     <row r="276" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A276" s="13"/>
       <c r="B276" s="13"/>
       <c r="D276" s="5"/>
-      <c r="I276" s="12"/>
-      <c r="J276" s="12"/>
-      <c r="K276" s="12"/>
-      <c r="L276" s="12"/>
-      <c r="M276" s="12"/>
-      <c r="N276" s="12"/>
-      <c r="O276" s="12"/>
+      <c r="I276" s="14"/>
+      <c r="J276" s="14"/>
+      <c r="K276" s="14"/>
+      <c r="L276" s="14"/>
+      <c r="M276" s="14"/>
+      <c r="N276" s="14"/>
+      <c r="O276" s="14"/>
     </row>
     <row r="277" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A277" s="13"/>
       <c r="B277" s="13"/>
       <c r="D277" s="5"/>
-      <c r="I277" s="12"/>
-      <c r="J277" s="12"/>
-      <c r="K277" s="12"/>
-      <c r="L277" s="12"/>
-      <c r="M277" s="12"/>
-      <c r="N277" s="12"/>
-      <c r="O277" s="12"/>
+      <c r="I277" s="14"/>
+      <c r="J277" s="14"/>
+      <c r="K277" s="14"/>
+      <c r="L277" s="14"/>
+      <c r="M277" s="14"/>
+      <c r="N277" s="14"/>
+      <c r="O277" s="14"/>
     </row>
     <row r="278" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A278" s="13"/>
       <c r="B278" s="13"/>
       <c r="D278" s="5"/>
-      <c r="I278" s="12"/>
-      <c r="J278" s="12"/>
-      <c r="K278" s="12"/>
-      <c r="L278" s="12"/>
-      <c r="M278" s="12"/>
-      <c r="N278" s="12"/>
-      <c r="O278" s="12"/>
+      <c r="I278" s="14"/>
+      <c r="J278" s="14"/>
+      <c r="K278" s="14"/>
+      <c r="L278" s="14"/>
+      <c r="M278" s="14"/>
+      <c r="N278" s="14"/>
+      <c r="O278" s="14"/>
     </row>
     <row r="279" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A279" s="13"/>
       <c r="B279" s="13"/>
       <c r="D279" s="5"/>
-      <c r="I279" s="12"/>
-      <c r="J279" s="12"/>
-      <c r="K279" s="12"/>
-      <c r="L279" s="12"/>
-      <c r="M279" s="12"/>
-      <c r="N279" s="12"/>
-      <c r="O279" s="12"/>
+      <c r="I279" s="14"/>
+      <c r="J279" s="14"/>
+      <c r="K279" s="14"/>
+      <c r="L279" s="14"/>
+      <c r="M279" s="14"/>
+      <c r="N279" s="14"/>
+      <c r="O279" s="14"/>
     </row>
     <row r="280" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A280" s="13"/>
       <c r="B280" s="13"/>
       <c r="D280" s="5"/>
-      <c r="I280" s="12"/>
-      <c r="J280" s="12"/>
-      <c r="K280" s="12"/>
-      <c r="L280" s="12"/>
-      <c r="M280" s="12"/>
-      <c r="N280" s="12"/>
-      <c r="O280" s="12"/>
+      <c r="I280" s="14"/>
+      <c r="J280" s="14"/>
+      <c r="K280" s="14"/>
+      <c r="L280" s="14"/>
+      <c r="M280" s="14"/>
+      <c r="N280" s="14"/>
+      <c r="O280" s="14"/>
     </row>
     <row r="281" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A281" s="13"/>
       <c r="B281" s="13"/>
       <c r="D281" s="5"/>
-      <c r="I281" s="12"/>
-      <c r="J281" s="12"/>
-      <c r="K281" s="12"/>
-      <c r="L281" s="12"/>
-      <c r="M281" s="12"/>
-      <c r="N281" s="12"/>
-      <c r="O281" s="12"/>
+      <c r="I281" s="14"/>
+      <c r="J281" s="14"/>
+      <c r="K281" s="14"/>
+      <c r="L281" s="14"/>
+      <c r="M281" s="14"/>
+      <c r="N281" s="14"/>
+      <c r="O281" s="14"/>
     </row>
     <row r="282" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A282" s="13"/>
       <c r="B282" s="13"/>
       <c r="D282" s="5"/>
-      <c r="I282" s="12"/>
-      <c r="J282" s="12"/>
-      <c r="K282" s="12"/>
-      <c r="L282" s="12"/>
-      <c r="M282" s="12"/>
-      <c r="N282" s="12"/>
-      <c r="O282" s="12"/>
+      <c r="I282" s="14"/>
+      <c r="J282" s="14"/>
+      <c r="K282" s="14"/>
+      <c r="L282" s="14"/>
+      <c r="M282" s="14"/>
+      <c r="N282" s="14"/>
+      <c r="O282" s="14"/>
     </row>
     <row r="283" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A283" s="13"/>
       <c r="B283" s="13"/>
       <c r="D283" s="5"/>
-      <c r="I283" s="12"/>
-      <c r="J283" s="12"/>
-      <c r="K283" s="12"/>
-      <c r="L283" s="12"/>
-      <c r="M283" s="12"/>
-      <c r="N283" s="12"/>
-      <c r="O283" s="12"/>
+      <c r="I283" s="14"/>
+      <c r="J283" s="14"/>
+      <c r="K283" s="14"/>
+      <c r="L283" s="14"/>
+      <c r="M283" s="14"/>
+      <c r="N283" s="14"/>
+      <c r="O283" s="14"/>
     </row>
     <row r="284" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A284" s="13"/>
       <c r="B284" s="13"/>
       <c r="D284" s="5"/>
-      <c r="I284" s="12"/>
-      <c r="J284" s="12"/>
-      <c r="K284" s="12"/>
-      <c r="L284" s="12"/>
-      <c r="M284" s="12"/>
-      <c r="N284" s="12"/>
-      <c r="O284" s="12"/>
+      <c r="I284" s="14"/>
+      <c r="J284" s="14"/>
+      <c r="K284" s="14"/>
+      <c r="L284" s="14"/>
+      <c r="M284" s="14"/>
+      <c r="N284" s="14"/>
+      <c r="O284" s="14"/>
     </row>
     <row r="285" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A285" s="13"/>
       <c r="B285" s="13"/>
       <c r="D285" s="5"/>
-      <c r="I285" s="12"/>
-      <c r="J285" s="12"/>
-      <c r="K285" s="12"/>
-      <c r="L285" s="12"/>
-      <c r="M285" s="12"/>
-      <c r="N285" s="12"/>
-      <c r="O285" s="12"/>
+      <c r="I285" s="14"/>
+      <c r="J285" s="14"/>
+      <c r="K285" s="14"/>
+      <c r="L285" s="14"/>
+      <c r="M285" s="14"/>
+      <c r="N285" s="14"/>
+      <c r="O285" s="14"/>
     </row>
     <row r="286" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A286" s="13"/>
       <c r="B286" s="13"/>
       <c r="D286" s="5"/>
-      <c r="I286" s="12"/>
-      <c r="J286" s="12"/>
-      <c r="K286" s="12"/>
-      <c r="L286" s="12"/>
-      <c r="M286" s="12"/>
-      <c r="N286" s="12"/>
-      <c r="O286" s="12"/>
+      <c r="I286" s="14"/>
+      <c r="J286" s="14"/>
+      <c r="K286" s="14"/>
+      <c r="L286" s="14"/>
+      <c r="M286" s="14"/>
+      <c r="N286" s="14"/>
+      <c r="O286" s="14"/>
     </row>
     <row r="287" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A287" s="13"/>
       <c r="B287" s="13"/>
       <c r="D287" s="5"/>
-      <c r="I287" s="12"/>
-      <c r="J287" s="12"/>
-      <c r="K287" s="12"/>
-      <c r="L287" s="12"/>
-      <c r="M287" s="12"/>
-      <c r="N287" s="12"/>
-      <c r="O287" s="12"/>
+      <c r="I287" s="14"/>
+      <c r="J287" s="14"/>
+      <c r="K287" s="14"/>
+      <c r="L287" s="14"/>
+      <c r="M287" s="14"/>
+      <c r="N287" s="14"/>
+      <c r="O287" s="14"/>
     </row>
     <row r="288" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A288" s="13"/>
       <c r="B288" s="13"/>
       <c r="D288" s="5"/>
-      <c r="I288" s="12"/>
-      <c r="J288" s="12"/>
-      <c r="K288" s="12"/>
-      <c r="L288" s="12"/>
-      <c r="M288" s="12"/>
-      <c r="N288" s="12"/>
-      <c r="O288" s="12"/>
+      <c r="I288" s="14"/>
+      <c r="J288" s="14"/>
+      <c r="K288" s="14"/>
+      <c r="L288" s="14"/>
+      <c r="M288" s="14"/>
+      <c r="N288" s="14"/>
+      <c r="O288" s="14"/>
     </row>
     <row r="289" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A289" s="13"/>
       <c r="B289" s="13"/>
       <c r="D289" s="5"/>
-      <c r="I289" s="12"/>
-      <c r="J289" s="12"/>
-      <c r="K289" s="12"/>
-      <c r="L289" s="12"/>
-      <c r="M289" s="12"/>
-      <c r="N289" s="12"/>
-      <c r="O289" s="12"/>
+      <c r="I289" s="14"/>
+      <c r="J289" s="14"/>
+      <c r="K289" s="14"/>
+      <c r="L289" s="14"/>
+      <c r="M289" s="14"/>
+      <c r="N289" s="14"/>
+      <c r="O289" s="14"/>
     </row>
     <row r="290" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A290" s="13"/>
       <c r="B290" s="13"/>
       <c r="D290" s="5"/>
-      <c r="I290" s="12"/>
-      <c r="J290" s="12"/>
-      <c r="K290" s="12"/>
-      <c r="L290" s="12"/>
-      <c r="M290" s="12"/>
-      <c r="N290" s="12"/>
-      <c r="O290" s="12"/>
+      <c r="I290" s="14"/>
+      <c r="J290" s="14"/>
+      <c r="K290" s="14"/>
+      <c r="L290" s="14"/>
+      <c r="M290" s="14"/>
+      <c r="N290" s="14"/>
+      <c r="O290" s="14"/>
     </row>
     <row r="291" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A291" s="13"/>
       <c r="B291" s="13"/>
       <c r="D291" s="5"/>
-      <c r="I291" s="12"/>
-      <c r="J291" s="12"/>
-      <c r="K291" s="12"/>
-      <c r="L291" s="12"/>
-      <c r="M291" s="12"/>
-      <c r="N291" s="12"/>
-      <c r="O291" s="12"/>
+      <c r="I291" s="14"/>
+      <c r="J291" s="14"/>
+      <c r="K291" s="14"/>
+      <c r="L291" s="14"/>
+      <c r="M291" s="14"/>
+      <c r="N291" s="14"/>
+      <c r="O291" s="14"/>
     </row>
     <row r="292" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A292" s="13"/>
       <c r="B292" s="13"/>
       <c r="D292" s="5"/>
-      <c r="I292" s="12"/>
-      <c r="J292" s="12"/>
-      <c r="K292" s="12"/>
-      <c r="L292" s="12"/>
-      <c r="M292" s="12"/>
-      <c r="N292" s="12"/>
-      <c r="O292" s="12"/>
+      <c r="I292" s="14"/>
+      <c r="J292" s="14"/>
+      <c r="K292" s="14"/>
+      <c r="L292" s="14"/>
+      <c r="M292" s="14"/>
+      <c r="N292" s="14"/>
+      <c r="O292" s="14"/>
     </row>
     <row r="293" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A293" s="13"/>
       <c r="B293" s="13"/>
       <c r="D293" s="5"/>
-      <c r="I293" s="12"/>
-      <c r="J293" s="12"/>
-      <c r="K293" s="12"/>
-      <c r="L293" s="12"/>
-      <c r="M293" s="12"/>
-      <c r="N293" s="12"/>
-      <c r="O293" s="12"/>
+      <c r="I293" s="14"/>
+      <c r="J293" s="14"/>
+      <c r="K293" s="14"/>
+      <c r="L293" s="14"/>
+      <c r="M293" s="14"/>
+      <c r="N293" s="14"/>
+      <c r="O293" s="14"/>
     </row>
     <row r="294" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A294" s="13"/>
       <c r="B294" s="13"/>
       <c r="D294" s="5"/>
-      <c r="I294" s="12"/>
-      <c r="J294" s="12"/>
-      <c r="K294" s="12"/>
-      <c r="L294" s="12"/>
-      <c r="M294" s="12"/>
-      <c r="N294" s="12"/>
-      <c r="O294" s="12"/>
+      <c r="I294" s="14"/>
+      <c r="J294" s="14"/>
+      <c r="K294" s="14"/>
+      <c r="L294" s="14"/>
+      <c r="M294" s="14"/>
+      <c r="N294" s="14"/>
+      <c r="O294" s="14"/>
     </row>
     <row r="295" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A295" s="13"/>
       <c r="B295" s="13"/>
       <c r="D295" s="5"/>
-      <c r="I295" s="12"/>
-      <c r="J295" s="12"/>
-      <c r="K295" s="12"/>
-      <c r="L295" s="12"/>
-      <c r="M295" s="12"/>
-      <c r="N295" s="12"/>
-      <c r="O295" s="12"/>
+      <c r="I295" s="14"/>
+      <c r="J295" s="14"/>
+      <c r="K295" s="14"/>
+      <c r="L295" s="14"/>
+      <c r="M295" s="14"/>
+      <c r="N295" s="14"/>
+      <c r="O295" s="14"/>
     </row>
     <row r="296" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A296" s="13"/>
       <c r="B296" s="13"/>
       <c r="D296" s="5"/>
-      <c r="I296" s="12"/>
-      <c r="J296" s="12"/>
-      <c r="K296" s="12"/>
-      <c r="L296" s="12"/>
-      <c r="M296" s="12"/>
-      <c r="N296" s="12"/>
-      <c r="O296" s="12"/>
+      <c r="I296" s="14"/>
+      <c r="J296" s="14"/>
+      <c r="K296" s="14"/>
+      <c r="L296" s="14"/>
+      <c r="M296" s="14"/>
+      <c r="N296" s="14"/>
+      <c r="O296" s="14"/>
     </row>
     <row r="297" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A297" s="13"/>
       <c r="B297" s="13"/>
       <c r="D297" s="5"/>
-      <c r="I297" s="12"/>
-      <c r="J297" s="12"/>
-      <c r="K297" s="12"/>
-      <c r="L297" s="12"/>
-      <c r="M297" s="12"/>
-      <c r="N297" s="12"/>
-      <c r="O297" s="12"/>
+      <c r="I297" s="14"/>
+      <c r="J297" s="14"/>
+      <c r="K297" s="14"/>
+      <c r="L297" s="14"/>
+      <c r="M297" s="14"/>
+      <c r="N297" s="14"/>
+      <c r="O297" s="14"/>
     </row>
     <row r="298" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A298" s="13"/>
       <c r="B298" s="13"/>
       <c r="D298" s="5"/>
-      <c r="I298" s="12"/>
-      <c r="J298" s="12"/>
-      <c r="K298" s="12"/>
-      <c r="L298" s="12"/>
-      <c r="M298" s="12"/>
-      <c r="N298" s="12"/>
-      <c r="O298" s="12"/>
+      <c r="I298" s="14"/>
+      <c r="J298" s="14"/>
+      <c r="K298" s="14"/>
+      <c r="L298" s="14"/>
+      <c r="M298" s="14"/>
+      <c r="N298" s="14"/>
+      <c r="O298" s="14"/>
     </row>
     <row r="299" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A299" s="13"/>
       <c r="B299" s="13"/>
       <c r="D299" s="5"/>
+      <c r="I299" s="14"/>
+      <c r="J299" s="14"/>
+      <c r="K299" s="14"/>
+      <c r="L299" s="14"/>
+      <c r="M299" s="14"/>
+      <c r="N299" s="14"/>
+      <c r="O299" s="14"/>
     </row>
     <row r="300" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A300" s="13"/>
@@ -5339,7 +5353,7 @@
       <c r="B426" s="13"/>
       <c r="D426" s="5"/>
     </row>
-    <row r="427" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="427" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A427" s="13"/>
       <c r="B427" s="13"/>
       <c r="D427" s="5"/>
@@ -5547,11 +5561,11 @@
     <row r="468" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A468" s="13"/>
       <c r="B468" s="13"/>
+      <c r="D468" s="5"/>
     </row>
     <row r="469" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A469" s="13"/>
       <c r="B469" s="13"/>
-      <c r="D469" s="5"/>
     </row>
     <row r="470" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A470" s="13"/>
@@ -5601,11 +5615,11 @@
     <row r="479" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A479" s="13"/>
       <c r="B479" s="13"/>
+      <c r="D479" s="5"/>
     </row>
     <row r="480" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A480" s="13"/>
       <c r="B480" s="13"/>
-      <c r="D480" s="5"/>
     </row>
     <row r="481" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A481" s="13"/>
@@ -5660,6 +5674,7 @@
     <row r="491" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A491" s="13"/>
       <c r="B491" s="13"/>
+      <c r="D491" s="5"/>
     </row>
     <row r="492" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A492" s="13"/>
@@ -5863,12 +5878,12 @@
     </row>
     <row r="542" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A542" s="13"/>
-      <c r="B542" s="10"/>
-      <c r="G542" s="11"/>
+      <c r="B542" s="13"/>
     </row>
     <row r="543" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A543" s="13"/>
       <c r="B543" s="10"/>
+      <c r="G543" s="11"/>
     </row>
     <row r="544" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A544" s="13"/>
@@ -6012,7 +6027,7 @@
     </row>
     <row r="579" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A579" s="13"/>
-      <c r="B579" s="13"/>
+      <c r="B579" s="10"/>
     </row>
     <row r="580" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A580" s="13"/>
@@ -6028,10 +6043,10 @@
     </row>
     <row r="583" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A583" s="13"/>
+      <c r="B583" s="13"/>
     </row>
     <row r="584" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A584" s="13"/>
-      <c r="B584" s="13"/>
     </row>
     <row r="585" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A585" s="13"/>
@@ -6055,10 +6070,10 @@
     </row>
     <row r="590" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A590" s="13"/>
+      <c r="B590" s="13"/>
     </row>
     <row r="591" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A591" s="13"/>
-      <c r="B591" s="13"/>
     </row>
     <row r="592" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A592" s="13"/>
@@ -6374,63 +6389,63 @@
     </row>
     <row r="670" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A670" s="13"/>
-      <c r="B670" s="15"/>
+      <c r="B670" s="13"/>
     </row>
     <row r="671" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A671" s="13"/>
-      <c r="B671" s="15"/>
+      <c r="B671" s="12"/>
     </row>
     <row r="672" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A672" s="13"/>
-      <c r="B672" s="15"/>
+      <c r="B672" s="12"/>
     </row>
     <row r="673" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A673" s="13"/>
-      <c r="B673" s="15"/>
+      <c r="B673" s="12"/>
     </row>
     <row r="674" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A674" s="13"/>
-      <c r="B674" s="15"/>
+      <c r="B674" s="12"/>
     </row>
     <row r="675" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A675" s="13"/>
-      <c r="B675" s="15"/>
+      <c r="B675" s="12"/>
     </row>
     <row r="676" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A676" s="13"/>
-      <c r="B676" s="15"/>
+      <c r="B676" s="12"/>
     </row>
     <row r="677" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A677" s="13"/>
-      <c r="B677" s="15"/>
+      <c r="B677" s="12"/>
     </row>
     <row r="678" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A678" s="13"/>
-      <c r="B678" s="15"/>
+      <c r="B678" s="12"/>
     </row>
     <row r="679" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A679" s="13"/>
-      <c r="B679" s="15"/>
+      <c r="B679" s="12"/>
     </row>
     <row r="680" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A680" s="13"/>
-      <c r="B680" s="15"/>
+      <c r="B680" s="12"/>
     </row>
     <row r="681" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A681" s="13"/>
-      <c r="B681" s="15"/>
+      <c r="B681" s="12"/>
     </row>
     <row r="682" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A682" s="13"/>
-      <c r="B682" s="15"/>
+      <c r="B682" s="12"/>
     </row>
     <row r="683" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A683" s="13"/>
-      <c r="B683" s="15"/>
+      <c r="B683" s="12"/>
     </row>
     <row r="684" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A684" s="13"/>
-      <c r="B684" s="13"/>
+      <c r="B684" s="12"/>
     </row>
     <row r="685" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A685" s="13"/>
@@ -6506,10 +6521,10 @@
     </row>
     <row r="703" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A703" s="13"/>
+      <c r="B703" s="13"/>
     </row>
     <row r="704" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A704" s="13"/>
-      <c r="B704" s="13"/>
     </row>
     <row r="705" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A705" s="13"/>
@@ -6533,14 +6548,14 @@
     </row>
     <row r="710" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A710" s="13"/>
+      <c r="B710" s="13"/>
     </row>
     <row r="711" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A711" s="13"/>
-      <c r="B711" s="15"/>
     </row>
     <row r="712" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A712" s="13"/>
-      <c r="B712" s="13"/>
+      <c r="B712" s="12"/>
     </row>
     <row r="713" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A713" s="13"/>
@@ -6556,11 +6571,11 @@
     </row>
     <row r="716" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A716" s="13"/>
-      <c r="B716" s="15"/>
+      <c r="B716" s="13"/>
     </row>
     <row r="717" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A717" s="13"/>
-      <c r="B717" s="13"/>
+      <c r="B717" s="12"/>
     </row>
     <row r="718" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A718" s="13"/>
@@ -6574,38 +6589,38 @@
       <c r="A720" s="13"/>
       <c r="B720" s="13"/>
     </row>
-    <row r="721" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="721" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A721" s="13"/>
-      <c r="B721" s="15"/>
-      <c r="H721" s="12" t="s">
+      <c r="B721" s="13"/>
+    </row>
+    <row r="722" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A722" s="13"/>
+      <c r="B722" s="12"/>
+      <c r="H722" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="722" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A722" s="13"/>
-      <c r="B722" s="15"/>
-      <c r="H722" s="12"/>
-    </row>
     <row r="723" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A723" s="13"/>
-      <c r="B723" s="15"/>
-      <c r="H723" s="12"/>
+      <c r="B723" s="12"/>
+      <c r="H723" s="14"/>
     </row>
     <row r="724" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A724" s="13"/>
-      <c r="B724" s="15"/>
+      <c r="B724" s="12"/>
+      <c r="H724" s="14"/>
     </row>
     <row r="725" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A725" s="13"/>
-      <c r="B725" s="15"/>
+      <c r="B725" s="12"/>
     </row>
     <row r="726" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A726" s="13"/>
-      <c r="B726" s="15"/>
+      <c r="B726" s="12"/>
     </row>
     <row r="727" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A727" s="13"/>
-      <c r="B727" s="6"/>
+      <c r="B727" s="12"/>
     </row>
     <row r="728" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A728" s="13"/>
@@ -6613,7 +6628,7 @@
     </row>
     <row r="729" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A729" s="13"/>
-      <c r="B729" s="13"/>
+      <c r="B729" s="6"/>
     </row>
     <row r="730" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A730" s="13"/>
@@ -6797,16 +6812,16 @@
     </row>
     <row r="775" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A775" s="13"/>
-      <c r="B775" s="15"/>
+      <c r="B775" s="13"/>
     </row>
     <row r="776" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A776" s="13"/>
-      <c r="B776" s="13"/>
-      <c r="K776" s="2"/>
+      <c r="B776" s="12"/>
     </row>
     <row r="777" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A777" s="13"/>
       <c r="B777" s="13"/>
+      <c r="K777" s="2"/>
     </row>
     <row r="778" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A778" s="13"/>
@@ -6927,7 +6942,6 @@
     <row r="807" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A807" s="13"/>
       <c r="B807" s="13"/>
-      <c r="K807" s="2"/>
     </row>
     <row r="808" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A808" s="13"/>
@@ -6946,12 +6960,12 @@
     </row>
     <row r="811" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A811" s="13"/>
-      <c r="B811" s="15"/>
+      <c r="B811" s="13"/>
       <c r="K811" s="2"/>
     </row>
     <row r="812" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A812" s="13"/>
-      <c r="B812" s="13"/>
+      <c r="B812" s="12"/>
       <c r="K812" s="2"/>
     </row>
     <row r="813" spans="1:11" x14ac:dyDescent="0.6">
@@ -6971,676 +6985,677 @@
     </row>
     <row r="816" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A816" s="13"/>
-      <c r="B816" s="15"/>
+      <c r="B816" s="13"/>
       <c r="K816" s="2"/>
     </row>
     <row r="817" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A817" s="13"/>
-      <c r="B817" s="15"/>
+      <c r="B817" s="12"/>
       <c r="K817" s="2"/>
     </row>
     <row r="818" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A818" s="13"/>
-      <c r="B818" s="15"/>
+      <c r="B818" s="12"/>
       <c r="K818" s="2"/>
     </row>
     <row r="819" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A819" s="13"/>
-      <c r="B819" s="15"/>
+      <c r="B819" s="12"/>
       <c r="K819" s="2"/>
     </row>
     <row r="820" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A820" s="13"/>
-      <c r="B820" s="15"/>
+      <c r="B820" s="12"/>
       <c r="K820" s="2"/>
     </row>
     <row r="821" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A821" s="13"/>
-      <c r="B821" s="15"/>
+      <c r="B821" s="12"/>
       <c r="K821" s="2"/>
     </row>
     <row r="822" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A822" s="13"/>
-      <c r="B822" s="15"/>
+      <c r="B822" s="12"/>
       <c r="K822" s="2"/>
     </row>
     <row r="823" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A823" s="13"/>
-      <c r="B823" s="15"/>
+      <c r="B823" s="12"/>
       <c r="K823" s="2"/>
     </row>
     <row r="824" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A824" s="13"/>
-      <c r="B824" s="15"/>
+      <c r="B824" s="12"/>
       <c r="K824" s="2"/>
     </row>
     <row r="825" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A825" s="13"/>
-      <c r="B825" s="15"/>
+      <c r="B825" s="12"/>
       <c r="K825" s="2"/>
     </row>
     <row r="826" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A826" s="13"/>
-      <c r="B826" s="15"/>
+      <c r="B826" s="12"/>
       <c r="K826" s="2"/>
     </row>
     <row r="827" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A827" s="13"/>
-      <c r="B827" s="15"/>
+      <c r="B827" s="12"/>
       <c r="K827" s="2"/>
     </row>
     <row r="828" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A828" s="13"/>
-      <c r="B828" s="15"/>
+      <c r="B828" s="12"/>
       <c r="K828" s="2"/>
     </row>
     <row r="829" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A829" s="13"/>
-      <c r="B829" s="15"/>
+      <c r="B829" s="12"/>
       <c r="K829" s="2"/>
     </row>
     <row r="830" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A830" s="13"/>
-      <c r="B830" s="15"/>
+      <c r="B830" s="12"/>
       <c r="K830" s="2"/>
     </row>
     <row r="831" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A831" s="13"/>
-      <c r="B831" s="15"/>
+      <c r="B831" s="12"/>
+      <c r="K831" s="2"/>
     </row>
     <row r="832" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A832" s="13"/>
-      <c r="B832" s="15"/>
+      <c r="B832" s="12"/>
     </row>
     <row r="833" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A833" s="13"/>
-      <c r="B833" s="15"/>
+      <c r="B833" s="12"/>
     </row>
     <row r="834" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A834" s="13"/>
-      <c r="B834" s="15"/>
+      <c r="B834" s="12"/>
     </row>
     <row r="835" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A835" s="13"/>
-      <c r="B835" s="15"/>
-      <c r="D835" s="3"/>
+      <c r="B835" s="12"/>
     </row>
     <row r="836" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A836" s="13"/>
-      <c r="B836" s="15"/>
+      <c r="B836" s="12"/>
       <c r="D836" s="3"/>
     </row>
     <row r="837" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A837" s="13"/>
-      <c r="B837" s="15"/>
+      <c r="B837" s="12"/>
       <c r="D837" s="3"/>
     </row>
     <row r="838" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A838" s="13"/>
-      <c r="B838" s="15"/>
+      <c r="B838" s="12"/>
       <c r="D838" s="3"/>
     </row>
     <row r="839" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A839" s="13"/>
-      <c r="B839" s="15"/>
+      <c r="B839" s="12"/>
       <c r="D839" s="3"/>
     </row>
     <row r="840" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A840" s="13"/>
-      <c r="B840" s="15"/>
+      <c r="B840" s="12"/>
       <c r="D840" s="3"/>
     </row>
     <row r="841" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A841" s="13"/>
-      <c r="B841" s="15"/>
+      <c r="B841" s="12"/>
       <c r="D841" s="3"/>
     </row>
     <row r="842" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A842" s="13"/>
-      <c r="B842" s="15"/>
+      <c r="B842" s="12"/>
+      <c r="D842" s="3"/>
     </row>
     <row r="843" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A843" s="13"/>
-      <c r="B843" s="15"/>
+      <c r="B843" s="12"/>
     </row>
     <row r="844" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A844" s="13"/>
-      <c r="B844" s="15"/>
+      <c r="B844" s="12"/>
     </row>
     <row r="845" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A845" s="13"/>
-      <c r="B845" s="15"/>
+      <c r="B845" s="12"/>
     </row>
     <row r="846" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A846" s="13"/>
-      <c r="B846" s="15"/>
+      <c r="B846" s="12"/>
     </row>
     <row r="847" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A847" s="13"/>
-      <c r="B847" s="15"/>
+      <c r="B847" s="12"/>
     </row>
     <row r="848" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A848" s="13"/>
-      <c r="B848" s="15"/>
+      <c r="B848" s="12"/>
     </row>
     <row r="849" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A849" s="13"/>
-      <c r="B849" s="15"/>
+      <c r="B849" s="12"/>
     </row>
     <row r="850" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A850" s="13"/>
-      <c r="B850" s="15"/>
+      <c r="B850" s="12"/>
     </row>
     <row r="851" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A851" s="13"/>
-      <c r="B851" s="15"/>
+      <c r="B851" s="12"/>
     </row>
     <row r="852" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A852" s="13"/>
-      <c r="B852" s="15"/>
+      <c r="B852" s="12"/>
     </row>
     <row r="853" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A853" s="13"/>
-      <c r="B853" s="15"/>
-      <c r="H853" s="2"/>
+      <c r="B853" s="12"/>
     </row>
     <row r="854" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A854" s="13"/>
-      <c r="B854" s="15"/>
+      <c r="B854" s="12"/>
       <c r="H854" s="2"/>
     </row>
     <row r="855" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A855" s="13"/>
-      <c r="B855" s="15"/>
+      <c r="B855" s="12"/>
       <c r="H855" s="2"/>
     </row>
     <row r="856" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A856" s="13"/>
-      <c r="B856" s="15"/>
+      <c r="B856" s="12"/>
       <c r="H856" s="2"/>
     </row>
     <row r="857" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A857" s="13"/>
-      <c r="B857" s="15"/>
+      <c r="B857" s="12"/>
       <c r="H857" s="2"/>
     </row>
     <row r="858" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A858" s="13"/>
-      <c r="B858" s="15"/>
+      <c r="B858" s="12"/>
       <c r="H858" s="2"/>
     </row>
     <row r="859" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A859" s="13"/>
-      <c r="B859" s="15"/>
+      <c r="B859" s="12"/>
       <c r="H859" s="2"/>
     </row>
     <row r="860" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A860" s="13"/>
-      <c r="B860" s="15"/>
+      <c r="B860" s="12"/>
       <c r="H860" s="2"/>
     </row>
     <row r="861" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A861" s="13"/>
-      <c r="B861" s="15"/>
+      <c r="B861" s="12"/>
       <c r="H861" s="2"/>
     </row>
     <row r="862" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A862" s="13"/>
-      <c r="B862" s="15"/>
+      <c r="B862" s="12"/>
       <c r="H862" s="2"/>
     </row>
     <row r="863" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A863" s="13"/>
-      <c r="B863" s="15"/>
+      <c r="B863" s="12"/>
       <c r="H863" s="2"/>
     </row>
     <row r="864" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A864" s="13"/>
-      <c r="B864" s="15"/>
+      <c r="B864" s="12"/>
       <c r="H864" s="2"/>
     </row>
-    <row r="865" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="865" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A865" s="13"/>
-      <c r="B865" s="15"/>
-    </row>
-    <row r="866" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B865" s="12"/>
+      <c r="H865" s="2"/>
+    </row>
+    <row r="866" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A866" s="13"/>
-      <c r="B866" s="15"/>
-    </row>
-    <row r="867" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B866" s="12"/>
+    </row>
+    <row r="867" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A867" s="13"/>
-      <c r="B867" s="15"/>
-    </row>
-    <row r="868" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B867" s="12"/>
+    </row>
+    <row r="868" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A868" s="13"/>
-      <c r="B868" s="15"/>
-    </row>
-    <row r="869" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B868" s="12"/>
+    </row>
+    <row r="869" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A869" s="13"/>
-      <c r="B869" s="15"/>
-    </row>
-    <row r="870" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B869" s="12"/>
+    </row>
+    <row r="870" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A870" s="13"/>
-      <c r="B870" s="15"/>
-    </row>
-    <row r="871" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B870" s="12"/>
+    </row>
+    <row r="871" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A871" s="13"/>
-      <c r="B871" s="15"/>
-    </row>
-    <row r="872" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B871" s="12"/>
+    </row>
+    <row r="872" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A872" s="13"/>
-      <c r="B872" s="15"/>
-    </row>
-    <row r="873" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B872" s="12"/>
+    </row>
+    <row r="873" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A873" s="13"/>
-      <c r="B873" s="15"/>
-    </row>
-    <row r="874" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B873" s="12"/>
+    </row>
+    <row r="874" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A874" s="13"/>
-      <c r="B874" s="15"/>
-    </row>
-    <row r="875" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B874" s="12"/>
+    </row>
+    <row r="875" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A875" s="13"/>
-      <c r="B875" s="15"/>
-    </row>
-    <row r="876" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B875" s="12"/>
+    </row>
+    <row r="876" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A876" s="13"/>
-      <c r="B876" s="15"/>
-    </row>
-    <row r="877" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B876" s="12"/>
+    </row>
+    <row r="877" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A877" s="13"/>
-      <c r="B877" s="15"/>
-    </row>
-    <row r="878" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B877" s="12"/>
+    </row>
+    <row r="878" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A878" s="13"/>
-      <c r="B878" s="15"/>
-    </row>
-    <row r="879" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B878" s="12"/>
+    </row>
+    <row r="879" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A879" s="13"/>
-      <c r="B879" s="15"/>
-    </row>
-    <row r="880" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B879" s="12"/>
+    </row>
+    <row r="880" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A880" s="13"/>
-      <c r="B880" s="15"/>
+      <c r="B880" s="12"/>
     </row>
     <row r="881" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A881" s="13"/>
-      <c r="B881" s="15"/>
+      <c r="B881" s="12"/>
     </row>
     <row r="882" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A882" s="13"/>
-      <c r="B882" s="15"/>
+      <c r="B882" s="12"/>
     </row>
     <row r="883" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A883" s="13"/>
-      <c r="B883" s="15"/>
+      <c r="B883" s="12"/>
     </row>
     <row r="884" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A884" s="13"/>
-      <c r="B884" s="15"/>
+      <c r="B884" s="12"/>
     </row>
     <row r="885" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A885" s="13"/>
-      <c r="B885" s="15"/>
+      <c r="B885" s="12"/>
     </row>
     <row r="886" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A886" s="13"/>
-      <c r="B886" s="15"/>
+      <c r="B886" s="12"/>
     </row>
     <row r="887" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A887" s="13"/>
-      <c r="B887" s="15"/>
+      <c r="B887" s="12"/>
     </row>
     <row r="888" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A888" s="13"/>
-      <c r="B888" s="15"/>
+      <c r="B888" s="12"/>
     </row>
     <row r="889" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A889" s="13"/>
-      <c r="B889" s="15"/>
+      <c r="B889" s="12"/>
     </row>
     <row r="890" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A890" s="13"/>
-      <c r="B890" s="15"/>
-      <c r="D890" s="3"/>
-      <c r="I890" s="2"/>
+      <c r="B890" s="12"/>
     </row>
     <row r="891" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A891" s="13"/>
-      <c r="B891" s="15"/>
+      <c r="B891" s="12"/>
       <c r="D891" s="3"/>
       <c r="I891" s="2"/>
     </row>
     <row r="892" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A892" s="13"/>
-      <c r="B892" s="15"/>
+      <c r="B892" s="12"/>
       <c r="D892" s="3"/>
       <c r="I892" s="2"/>
     </row>
     <row r="893" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A893" s="13"/>
-      <c r="B893" s="15"/>
+      <c r="B893" s="12"/>
       <c r="D893" s="3"/>
       <c r="I893" s="2"/>
     </row>
     <row r="894" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A894" s="13"/>
-      <c r="B894" s="15"/>
+      <c r="B894" s="12"/>
       <c r="D894" s="3"/>
       <c r="I894" s="2"/>
     </row>
     <row r="895" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A895" s="13"/>
-      <c r="B895" s="15"/>
+      <c r="B895" s="12"/>
       <c r="D895" s="3"/>
       <c r="I895" s="2"/>
     </row>
     <row r="896" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A896" s="13"/>
-      <c r="B896" s="15"/>
+      <c r="B896" s="12"/>
+      <c r="D896" s="3"/>
       <c r="I896" s="2"/>
     </row>
     <row r="897" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A897" s="13"/>
-      <c r="B897" s="15"/>
+      <c r="B897" s="12"/>
       <c r="I897" s="2"/>
     </row>
     <row r="898" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A898" s="13"/>
-      <c r="B898" s="15"/>
+      <c r="B898" s="12"/>
       <c r="I898" s="2"/>
     </row>
     <row r="899" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A899" s="13"/>
-      <c r="B899" s="15"/>
+      <c r="B899" s="12"/>
       <c r="I899" s="2"/>
     </row>
     <row r="900" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A900" s="13"/>
-      <c r="B900" s="15"/>
+      <c r="B900" s="12"/>
       <c r="I900" s="2"/>
     </row>
     <row r="901" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A901" s="13"/>
-      <c r="B901" s="15"/>
+      <c r="B901" s="12"/>
       <c r="I901" s="2"/>
     </row>
     <row r="902" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A902" s="13"/>
-      <c r="B902" s="15"/>
+      <c r="B902" s="12"/>
       <c r="I902" s="2"/>
     </row>
     <row r="903" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A903" s="13"/>
-      <c r="B903" s="15"/>
+      <c r="B903" s="12"/>
       <c r="I903" s="2"/>
     </row>
     <row r="904" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A904" s="13"/>
-      <c r="B904" s="15"/>
+      <c r="B904" s="12"/>
       <c r="I904" s="2"/>
     </row>
     <row r="905" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A905" s="13"/>
-      <c r="B905" s="15"/>
+      <c r="B905" s="12"/>
       <c r="I905" s="2"/>
     </row>
     <row r="906" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A906" s="13"/>
-      <c r="B906" s="15"/>
+      <c r="B906" s="12"/>
       <c r="I906" s="2"/>
     </row>
     <row r="907" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A907" s="13"/>
-      <c r="B907" s="15"/>
+      <c r="B907" s="12"/>
       <c r="I907" s="2"/>
     </row>
     <row r="908" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A908" s="13"/>
-      <c r="B908" s="15"/>
+      <c r="B908" s="12"/>
       <c r="I908" s="2"/>
     </row>
     <row r="909" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A909" s="13"/>
-      <c r="B909" s="15"/>
+      <c r="B909" s="12"/>
       <c r="I909" s="2"/>
     </row>
     <row r="910" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A910" s="13"/>
-      <c r="B910" s="15"/>
+      <c r="B910" s="12"/>
       <c r="I910" s="2"/>
     </row>
     <row r="911" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A911" s="13"/>
-      <c r="B911" s="15"/>
+      <c r="B911" s="12"/>
       <c r="I911" s="2"/>
     </row>
     <row r="912" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A912" s="13"/>
-      <c r="B912" s="15"/>
+      <c r="B912" s="12"/>
+      <c r="I912" s="2"/>
     </row>
     <row r="913" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A913" s="13"/>
-      <c r="B913" s="15"/>
+      <c r="B913" s="12"/>
     </row>
     <row r="914" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A914" s="13"/>
-      <c r="B914" s="15"/>
+      <c r="B914" s="12"/>
     </row>
     <row r="915" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A915" s="13"/>
-      <c r="B915" s="15"/>
+      <c r="B915" s="12"/>
     </row>
     <row r="916" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A916" s="13"/>
-      <c r="B916" s="15"/>
+      <c r="B916" s="12"/>
     </row>
     <row r="917" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A917" s="13"/>
-      <c r="B917" s="15"/>
+      <c r="B917" s="12"/>
     </row>
     <row r="918" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A918" s="13"/>
-      <c r="B918" s="15"/>
+      <c r="B918" s="12"/>
     </row>
     <row r="919" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A919" s="13"/>
-      <c r="B919" s="15"/>
+      <c r="B919" s="12"/>
     </row>
     <row r="920" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A920" s="13"/>
-      <c r="B920" s="15"/>
+      <c r="B920" s="12"/>
     </row>
     <row r="921" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A921" s="13"/>
-      <c r="B921" s="15"/>
-    </row>
-    <row r="922" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B921" s="12"/>
+    </row>
+    <row r="922" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A922" s="13"/>
-      <c r="B922" s="15"/>
-    </row>
-    <row r="923" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="B922" s="12"/>
+    </row>
+    <row r="923" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A923" s="13"/>
-      <c r="B923" s="15"/>
+      <c r="B923" s="12"/>
     </row>
     <row r="924" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A924" s="13"/>
-      <c r="B924" s="15"/>
+      <c r="B924" s="12"/>
     </row>
     <row r="925" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A925" s="13"/>
-      <c r="B925" s="15"/>
+      <c r="B925" s="12"/>
     </row>
     <row r="926" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A926" s="13"/>
-      <c r="B926" s="15"/>
+      <c r="B926" s="12"/>
     </row>
     <row r="927" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A927" s="13"/>
-      <c r="B927" s="15"/>
+      <c r="B927" s="12"/>
     </row>
     <row r="928" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A928" s="13"/>
-      <c r="B928" s="15"/>
+      <c r="B928" s="12"/>
     </row>
     <row r="929" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A929" s="13"/>
-      <c r="B929" s="15"/>
+      <c r="B929" s="12"/>
     </row>
     <row r="930" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A930" s="13"/>
-      <c r="B930" s="15"/>
+      <c r="B930" s="12"/>
     </row>
     <row r="931" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A931" s="13"/>
-      <c r="B931" s="15"/>
+      <c r="B931" s="12"/>
     </row>
     <row r="932" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A932" s="13"/>
-      <c r="B932" s="15"/>
+      <c r="B932" s="12"/>
     </row>
     <row r="933" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A933" s="13"/>
-      <c r="B933" s="15"/>
+      <c r="B933" s="12"/>
     </row>
     <row r="934" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A934" s="13"/>
-      <c r="B934" s="15"/>
+      <c r="B934" s="12"/>
     </row>
     <row r="935" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A935" s="13"/>
-      <c r="B935" s="15"/>
+      <c r="B935" s="12"/>
     </row>
     <row r="936" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A936" s="13"/>
-      <c r="B936" s="15"/>
-      <c r="H936" s="2"/>
+      <c r="B936" s="12"/>
     </row>
     <row r="937" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A937" s="13"/>
-      <c r="B937" s="15"/>
+      <c r="B937" s="12"/>
       <c r="H937" s="2"/>
     </row>
     <row r="938" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A938" s="13"/>
-      <c r="B938" s="15"/>
+      <c r="B938" s="12"/>
       <c r="H938" s="2"/>
     </row>
     <row r="939" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A939" s="13"/>
-      <c r="B939" s="15"/>
+      <c r="B939" s="12"/>
       <c r="H939" s="2"/>
     </row>
     <row r="940" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A940" s="13"/>
-      <c r="B940" s="15"/>
+      <c r="B940" s="12"/>
       <c r="H940" s="2"/>
     </row>
     <row r="941" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A941" s="13"/>
-      <c r="B941" s="15"/>
+      <c r="B941" s="12"/>
       <c r="H941" s="2"/>
     </row>
     <row r="942" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A942" s="13"/>
-      <c r="B942" s="15"/>
+      <c r="B942" s="12"/>
       <c r="H942" s="2"/>
     </row>
     <row r="943" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A943" s="13"/>
-      <c r="B943" s="15"/>
+      <c r="B943" s="12"/>
       <c r="H943" s="2"/>
     </row>
     <row r="944" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A944" s="13"/>
-      <c r="B944" s="13"/>
+      <c r="B944" s="12"/>
+      <c r="H944" s="2"/>
     </row>
     <row r="945" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A945" s="13"/>
+      <c r="B945" s="13"/>
     </row>
     <row r="946" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A946" s="13"/>
-      <c r="B946" s="15"/>
     </row>
     <row r="947" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A947" s="13"/>
-      <c r="B947" s="15"/>
+      <c r="B947" s="12"/>
     </row>
     <row r="948" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A948" s="13"/>
-      <c r="B948" s="15"/>
+      <c r="B948" s="12"/>
     </row>
     <row r="949" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A949" s="13"/>
-      <c r="B949" s="15"/>
+      <c r="B949" s="12"/>
     </row>
     <row r="950" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A950" s="13"/>
-      <c r="B950" s="15"/>
+      <c r="B950" s="12"/>
     </row>
     <row r="951" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A951" s="13"/>
-      <c r="B951" s="15"/>
+      <c r="B951" s="12"/>
     </row>
     <row r="952" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A952" s="13"/>
-      <c r="B952" s="15"/>
+      <c r="B952" s="12"/>
     </row>
     <row r="953" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A953" s="13"/>
-      <c r="B953" s="15"/>
+      <c r="B953" s="12"/>
     </row>
     <row r="954" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A954" s="13"/>
-      <c r="B954" s="15"/>
+      <c r="B954" s="12"/>
     </row>
     <row r="955" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A955" s="13"/>
-      <c r="B955" s="15"/>
+      <c r="B955" s="12"/>
     </row>
     <row r="956" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A956" s="13"/>
-      <c r="B956" s="15"/>
+      <c r="B956" s="12"/>
     </row>
     <row r="957" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A957" s="13"/>
-      <c r="B957" s="15"/>
+      <c r="B957" s="12"/>
     </row>
     <row r="958" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A958" s="13"/>
-      <c r="B958" s="15"/>
+      <c r="B958" s="12"/>
     </row>
     <row r="959" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A959" s="13"/>
-      <c r="B959" s="15"/>
+      <c r="B959" s="12"/>
     </row>
     <row r="960" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A960" s="13"/>
-      <c r="B960" s="15"/>
+      <c r="B960" s="12"/>
     </row>
     <row r="961" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A961" s="13"/>
-      <c r="B961" s="15"/>
+      <c r="B961" s="12"/>
     </row>
     <row r="962" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A962" s="13"/>
-      <c r="B962" s="15"/>
+      <c r="B962" s="12"/>
     </row>
     <row r="963" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A963" s="13"/>
-      <c r="B963" s="15"/>
+      <c r="B963" s="12"/>
     </row>
     <row r="964" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A964" s="13"/>
-      <c r="B964" s="15"/>
+      <c r="B964" s="12"/>
     </row>
     <row r="965" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A965" s="13"/>
-      <c r="B965" s="15"/>
+      <c r="B965" s="12"/>
     </row>
     <row r="966" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A966" s="13"/>
-      <c r="B966" s="13"/>
+      <c r="B966" s="12"/>
     </row>
     <row r="967" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A967" s="13"/>
@@ -7666,11 +7681,11 @@
       <c r="A972" s="13"/>
       <c r="B972" s="13"/>
     </row>
-    <row r="973" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="973" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A973" s="13"/>
       <c r="B973" s="13"/>
     </row>
-    <row r="974" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="974" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A974" s="13"/>
       <c r="B974" s="13"/>
     </row>
@@ -7678,11 +7693,11 @@
       <c r="A975" s="13"/>
       <c r="B975" s="13"/>
     </row>
-    <row r="976" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="976" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A976" s="13"/>
       <c r="B976" s="13"/>
     </row>
-    <row r="977" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="977" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A977" s="13"/>
       <c r="B977" s="13"/>
     </row>
@@ -7716,86 +7731,85 @@
     </row>
     <row r="985" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A985" s="13"/>
-      <c r="B985" s="15"/>
+      <c r="B985" s="13"/>
     </row>
     <row r="986" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A986" s="13"/>
-      <c r="B986" s="15"/>
-      <c r="H986" s="2"/>
+      <c r="B986" s="12"/>
     </row>
     <row r="987" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A987" s="13"/>
-      <c r="B987" s="15"/>
+      <c r="B987" s="12"/>
       <c r="H987" s="2"/>
     </row>
     <row r="988" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A988" s="13"/>
-      <c r="B988" s="15"/>
+      <c r="B988" s="12"/>
       <c r="H988" s="2"/>
     </row>
     <row r="989" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A989" s="13"/>
-      <c r="B989" s="15"/>
+      <c r="B989" s="12"/>
       <c r="H989" s="2"/>
     </row>
     <row r="990" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A990" s="13"/>
-      <c r="B990" s="15"/>
+      <c r="B990" s="12"/>
       <c r="H990" s="2"/>
     </row>
     <row r="991" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A991" s="13"/>
-      <c r="B991" s="15"/>
+      <c r="B991" s="12"/>
       <c r="H991" s="2"/>
     </row>
     <row r="992" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A992" s="13"/>
-      <c r="B992" s="15"/>
+      <c r="B992" s="12"/>
       <c r="H992" s="2"/>
     </row>
     <row r="993" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A993" s="13"/>
-      <c r="B993" s="15"/>
+      <c r="B993" s="12"/>
       <c r="H993" s="2"/>
     </row>
     <row r="994" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A994" s="13"/>
-      <c r="B994" s="15"/>
+      <c r="B994" s="12"/>
       <c r="H994" s="2"/>
     </row>
     <row r="995" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A995" s="13"/>
-      <c r="B995" s="15"/>
+      <c r="B995" s="12"/>
       <c r="H995" s="2"/>
     </row>
     <row r="996" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A996" s="13"/>
-      <c r="B996" s="15"/>
+      <c r="B996" s="12"/>
       <c r="H996" s="2"/>
     </row>
     <row r="997" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A997" s="13"/>
-      <c r="B997" s="15"/>
+      <c r="B997" s="12"/>
       <c r="H997" s="2"/>
     </row>
     <row r="998" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A998" s="13"/>
-      <c r="B998" s="15"/>
+      <c r="B998" s="12"/>
       <c r="H998" s="2"/>
     </row>
     <row r="999" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A999" s="13"/>
-      <c r="B999" s="15"/>
+      <c r="B999" s="12"/>
       <c r="H999" s="2"/>
     </row>
     <row r="1000" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1000" s="13"/>
-      <c r="B1000" s="15"/>
+      <c r="B1000" s="12"/>
       <c r="H1000" s="2"/>
     </row>
     <row r="1001" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1001" s="13"/>
-      <c r="B1001" s="13"/>
+      <c r="B1001" s="12"/>
       <c r="H1001" s="2"/>
     </row>
     <row r="1002" spans="1:8" x14ac:dyDescent="0.6">
@@ -7815,6 +7829,7 @@
     </row>
     <row r="1005" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1005" s="13"/>
+      <c r="B1005" s="13"/>
       <c r="H1005" s="2"/>
     </row>
     <row r="1006" spans="1:8" x14ac:dyDescent="0.6">
@@ -7823,7 +7838,6 @@
     </row>
     <row r="1007" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1007" s="13"/>
-      <c r="B1007" s="13"/>
       <c r="H1007" s="2"/>
     </row>
     <row r="1008" spans="1:8" x14ac:dyDescent="0.6">
@@ -7853,77 +7867,77 @@
     </row>
     <row r="1013" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1013" s="13"/>
-      <c r="B1013" s="15"/>
+      <c r="B1013" s="13"/>
       <c r="H1013" s="2"/>
     </row>
     <row r="1014" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1014" s="13"/>
-      <c r="B1014" s="15"/>
+      <c r="B1014" s="12"/>
       <c r="H1014" s="2"/>
     </row>
     <row r="1015" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1015" s="13"/>
-      <c r="B1015" s="15"/>
+      <c r="B1015" s="12"/>
       <c r="H1015" s="2"/>
     </row>
     <row r="1016" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1016" s="13"/>
-      <c r="B1016" s="15"/>
+      <c r="B1016" s="12"/>
       <c r="H1016" s="2"/>
     </row>
     <row r="1017" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1017" s="13"/>
-      <c r="B1017" s="15"/>
+      <c r="B1017" s="12"/>
       <c r="H1017" s="2"/>
     </row>
     <row r="1018" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1018" s="13"/>
-      <c r="B1018" s="15"/>
+      <c r="B1018" s="12"/>
       <c r="H1018" s="2"/>
     </row>
     <row r="1019" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1019" s="13"/>
-      <c r="B1019" s="15"/>
+      <c r="B1019" s="12"/>
       <c r="H1019" s="2"/>
     </row>
     <row r="1020" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1020" s="13"/>
-      <c r="B1020" s="15"/>
+      <c r="B1020" s="12"/>
       <c r="H1020" s="2"/>
     </row>
     <row r="1021" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1021" s="13"/>
-      <c r="B1021" s="15"/>
+      <c r="B1021" s="12"/>
       <c r="H1021" s="2"/>
     </row>
     <row r="1022" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1022" s="13"/>
-      <c r="B1022" s="15"/>
+      <c r="B1022" s="12"/>
       <c r="H1022" s="2"/>
     </row>
     <row r="1023" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1023" s="13"/>
-      <c r="B1023" s="15"/>
+      <c r="B1023" s="12"/>
       <c r="H1023" s="2"/>
     </row>
     <row r="1024" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1024" s="13"/>
-      <c r="B1024" s="15"/>
+      <c r="B1024" s="12"/>
       <c r="H1024" s="2"/>
     </row>
     <row r="1025" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1025" s="13"/>
-      <c r="B1025" s="15"/>
+      <c r="B1025" s="12"/>
       <c r="H1025" s="2"/>
     </row>
     <row r="1026" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1026" s="13"/>
-      <c r="B1026" s="15"/>
+      <c r="B1026" s="12"/>
       <c r="H1026" s="2"/>
     </row>
     <row r="1027" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1027" s="13"/>
-      <c r="B1027" s="13"/>
+      <c r="B1027" s="12"/>
       <c r="H1027" s="2"/>
     </row>
     <row r="1028" spans="1:8" x14ac:dyDescent="0.6">
@@ -8126,9 +8140,10 @@
       <c r="B1067" s="13"/>
       <c r="H1067" s="2"/>
     </row>
-    <row r="1068" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1068" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1068" s="13"/>
       <c r="B1068" s="13"/>
+      <c r="H1068" s="2"/>
     </row>
     <row r="1069" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1069" s="13"/>
@@ -8170,7 +8185,7 @@
       <c r="A1078" s="13"/>
       <c r="B1078" s="13"/>
     </row>
-    <row r="1079" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="1079" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1079" s="13"/>
       <c r="B1079" s="13"/>
     </row>
@@ -8369,11 +8384,11 @@
     <row r="1128" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1128" s="13"/>
       <c r="B1128" s="13"/>
-      <c r="H1128" s="2"/>
     </row>
     <row r="1129" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1129" s="13"/>
       <c r="B1129" s="13"/>
+      <c r="H1129" s="2"/>
     </row>
     <row r="1130" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1130" s="13"/>
@@ -8387,11 +8402,11 @@
       <c r="A1132" s="13"/>
       <c r="B1132" s="13"/>
     </row>
-    <row r="1133" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1133" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1133" s="13"/>
       <c r="B1133" s="13"/>
     </row>
-    <row r="1134" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="1134" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1134" s="13"/>
       <c r="B1134" s="13"/>
     </row>
@@ -8803,11 +8818,11 @@
       <c r="A1236" s="13"/>
       <c r="B1236" s="13"/>
     </row>
-    <row r="1237" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1237" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A1237" s="13"/>
       <c r="B1237" s="13"/>
     </row>
-    <row r="1238" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="1238" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1238" s="13"/>
       <c r="B1238" s="13"/>
     </row>
@@ -8827,11 +8842,11 @@
       <c r="A1242" s="13"/>
       <c r="B1242" s="13"/>
     </row>
-    <row r="1243" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1243" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A1243" s="13"/>
       <c r="B1243" s="13"/>
     </row>
-    <row r="1244" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="1244" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1244" s="13"/>
       <c r="B1244" s="13"/>
     </row>
@@ -8877,6 +8892,7 @@
     </row>
     <row r="1255" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A1255" s="13"/>
+      <c r="B1255" s="13"/>
     </row>
     <row r="1256" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A1256" s="13"/>
@@ -8905,10 +8921,10 @@
     <row r="1264" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A1264" s="13"/>
     </row>
-    <row r="1265" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1265" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A1265" s="13"/>
     </row>
-    <row r="1266" spans="1:1" x14ac:dyDescent="0.6">
+    <row r="1266" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1266" s="13"/>
     </row>
     <row r="1267" spans="1:1" x14ac:dyDescent="0.6">
@@ -9631,80 +9647,83 @@
     <row r="1506" spans="1:1" x14ac:dyDescent="0.6">
       <c r="A1506" s="13"/>
     </row>
+    <row r="1507" spans="1:1" x14ac:dyDescent="0.6">
+      <c r="A1507" s="13"/>
+    </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="B965:B984"/>
-    <mergeCell ref="B778:B781"/>
-    <mergeCell ref="B997:B999"/>
-    <mergeCell ref="B991:B996"/>
-    <mergeCell ref="B535:B541"/>
-    <mergeCell ref="B985:B990"/>
-    <mergeCell ref="B933:B942"/>
-    <mergeCell ref="B721:B723"/>
-    <mergeCell ref="B901:B932"/>
-    <mergeCell ref="B881:B900"/>
-    <mergeCell ref="B811:B815"/>
-    <mergeCell ref="B818:B825"/>
-    <mergeCell ref="B816:B817"/>
-    <mergeCell ref="B946:B964"/>
-    <mergeCell ref="B943:B944"/>
-    <mergeCell ref="B826:B880"/>
-    <mergeCell ref="B782:B810"/>
-    <mergeCell ref="B729:B774"/>
-    <mergeCell ref="A956:A962"/>
-    <mergeCell ref="A981:A1506"/>
-    <mergeCell ref="B1094:B1254"/>
-    <mergeCell ref="A979:A980"/>
-    <mergeCell ref="A973:A978"/>
-    <mergeCell ref="A963:A972"/>
-    <mergeCell ref="B1080:B1083"/>
-    <mergeCell ref="B1067:B1079"/>
-    <mergeCell ref="B1026:B1028"/>
-    <mergeCell ref="B1092:B1093"/>
-    <mergeCell ref="B1084:B1091"/>
-    <mergeCell ref="B1057:B1066"/>
-    <mergeCell ref="B1029:B1056"/>
-    <mergeCell ref="B1013:B1025"/>
-    <mergeCell ref="B1007:B1012"/>
-    <mergeCell ref="B1000:B1004"/>
-    <mergeCell ref="A4:A955"/>
-    <mergeCell ref="B704:B709"/>
-    <mergeCell ref="B227:B377"/>
-    <mergeCell ref="B700:B702"/>
-    <mergeCell ref="B487:B509"/>
-    <mergeCell ref="B510:B530"/>
-    <mergeCell ref="B531:B534"/>
-    <mergeCell ref="B692:B699"/>
-    <mergeCell ref="B584:B585"/>
-    <mergeCell ref="B660:B669"/>
-    <mergeCell ref="B775:B777"/>
-    <mergeCell ref="B711:B715"/>
-    <mergeCell ref="B716:B720"/>
-    <mergeCell ref="B724:B726"/>
-    <mergeCell ref="I50:M110"/>
-    <mergeCell ref="B42:B53"/>
-    <mergeCell ref="B613:B632"/>
-    <mergeCell ref="B579:B582"/>
-    <mergeCell ref="B684:B691"/>
-    <mergeCell ref="B601:B612"/>
-    <mergeCell ref="B591:B600"/>
-    <mergeCell ref="B633:B659"/>
-    <mergeCell ref="B586:B589"/>
-    <mergeCell ref="B670:B683"/>
-    <mergeCell ref="B79:B180"/>
-    <mergeCell ref="B181:B226"/>
-    <mergeCell ref="B54:B78"/>
-    <mergeCell ref="H4:H9"/>
-    <mergeCell ref="H18:H26"/>
-    <mergeCell ref="H37:H41"/>
-    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="H722:H724"/>
+    <mergeCell ref="B470:B487"/>
+    <mergeCell ref="I228:O259"/>
+    <mergeCell ref="I260:O265"/>
+    <mergeCell ref="I266:O299"/>
+    <mergeCell ref="B379:B469"/>
+    <mergeCell ref="H4:H10"/>
+    <mergeCell ref="H19:H27"/>
+    <mergeCell ref="H38:H42"/>
+    <mergeCell ref="H28:H32"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="H721:H723"/>
-    <mergeCell ref="B469:B486"/>
-    <mergeCell ref="I227:O258"/>
-    <mergeCell ref="I259:O264"/>
-    <mergeCell ref="I265:O298"/>
-    <mergeCell ref="B378:B468"/>
+    <mergeCell ref="I51:M111"/>
+    <mergeCell ref="B43:B54"/>
+    <mergeCell ref="B614:B633"/>
+    <mergeCell ref="B580:B583"/>
+    <mergeCell ref="B685:B692"/>
+    <mergeCell ref="B602:B613"/>
+    <mergeCell ref="B592:B601"/>
+    <mergeCell ref="B634:B660"/>
+    <mergeCell ref="B587:B590"/>
+    <mergeCell ref="B671:B684"/>
+    <mergeCell ref="B80:B181"/>
+    <mergeCell ref="B182:B227"/>
+    <mergeCell ref="B55:B79"/>
+    <mergeCell ref="B1008:B1013"/>
+    <mergeCell ref="B1001:B1005"/>
+    <mergeCell ref="A4:A956"/>
+    <mergeCell ref="B705:B710"/>
+    <mergeCell ref="B228:B378"/>
+    <mergeCell ref="B701:B703"/>
+    <mergeCell ref="B488:B510"/>
+    <mergeCell ref="B511:B531"/>
+    <mergeCell ref="B532:B535"/>
+    <mergeCell ref="B693:B700"/>
+    <mergeCell ref="B585:B586"/>
+    <mergeCell ref="B661:B670"/>
+    <mergeCell ref="B776:B778"/>
+    <mergeCell ref="B712:B716"/>
+    <mergeCell ref="B717:B721"/>
+    <mergeCell ref="B725:B727"/>
+    <mergeCell ref="B783:B811"/>
+    <mergeCell ref="B730:B775"/>
+    <mergeCell ref="A957:A963"/>
+    <mergeCell ref="A982:A1507"/>
+    <mergeCell ref="B1095:B1255"/>
+    <mergeCell ref="A980:A981"/>
+    <mergeCell ref="A974:A979"/>
+    <mergeCell ref="A964:A973"/>
+    <mergeCell ref="B1081:B1084"/>
+    <mergeCell ref="B1068:B1080"/>
+    <mergeCell ref="B1027:B1029"/>
+    <mergeCell ref="B1093:B1094"/>
+    <mergeCell ref="B1085:B1092"/>
+    <mergeCell ref="B1058:B1067"/>
+    <mergeCell ref="B1030:B1057"/>
+    <mergeCell ref="B1014:B1026"/>
+    <mergeCell ref="B966:B985"/>
+    <mergeCell ref="B779:B782"/>
+    <mergeCell ref="B998:B1000"/>
+    <mergeCell ref="B992:B997"/>
+    <mergeCell ref="B536:B542"/>
+    <mergeCell ref="B986:B991"/>
+    <mergeCell ref="B934:B943"/>
+    <mergeCell ref="B722:B724"/>
+    <mergeCell ref="B902:B933"/>
+    <mergeCell ref="B882:B901"/>
+    <mergeCell ref="B812:B816"/>
+    <mergeCell ref="B819:B826"/>
+    <mergeCell ref="B817:B818"/>
+    <mergeCell ref="B947:B965"/>
+    <mergeCell ref="B944:B945"/>
+    <mergeCell ref="B827:B881"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C3">
@@ -9717,105 +9736,105 @@
     <cfRule type="duplicateValues" dxfId="153" priority="22"/>
     <cfRule type="duplicateValues" dxfId="152" priority="23"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C8">
+  <conditionalFormatting sqref="C4:C9">
     <cfRule type="duplicateValues" dxfId="151" priority="14748"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C181:C469 C471 C473 C475 C477:C478 C480 C482 C484 C486">
+  <conditionalFormatting sqref="C182:C470 C472 C474 C476 C478:C479 C481 C483 C485 C487">
     <cfRule type="duplicateValues" dxfId="150" priority="14678"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C506:C570">
+  <conditionalFormatting sqref="C507:C571">
     <cfRule type="duplicateValues" dxfId="149" priority="9454"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C571:C573">
+  <conditionalFormatting sqref="C572:C574">
     <cfRule type="duplicateValues" dxfId="148" priority="106"/>
     <cfRule type="duplicateValues" dxfId="147" priority="107"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C679:C686">
+  <conditionalFormatting sqref="C680:C687">
     <cfRule type="duplicateValues" dxfId="146" priority="5969"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C688">
+  <conditionalFormatting sqref="C689">
     <cfRule type="duplicateValues" dxfId="145" priority="185"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C695 C697">
+  <conditionalFormatting sqref="C696 C698">
     <cfRule type="duplicateValues" dxfId="144" priority="184"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C705">
+  <conditionalFormatting sqref="C706">
     <cfRule type="duplicateValues" dxfId="143" priority="159"/>
     <cfRule type="duplicateValues" dxfId="142" priority="160"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C752">
+  <conditionalFormatting sqref="C753">
     <cfRule type="duplicateValues" dxfId="141" priority="156"/>
     <cfRule type="duplicateValues" dxfId="140" priority="157"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C763">
+  <conditionalFormatting sqref="C764">
     <cfRule type="duplicateValues" dxfId="139" priority="119"/>
     <cfRule type="duplicateValues" dxfId="138" priority="120"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C764 C766:C767">
+  <conditionalFormatting sqref="C765 C767:C768">
     <cfRule type="duplicateValues" dxfId="137" priority="116"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C764">
+  <conditionalFormatting sqref="C765">
     <cfRule type="duplicateValues" dxfId="136" priority="117"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C765:C767">
+  <conditionalFormatting sqref="C766:C768">
     <cfRule type="duplicateValues" dxfId="135" priority="122"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C767">
+  <conditionalFormatting sqref="C768">
     <cfRule type="duplicateValues" dxfId="134" priority="123"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C856:C875">
+  <conditionalFormatting sqref="C857:C876">
     <cfRule type="duplicateValues" dxfId="133" priority="7424"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C896:C927">
+  <conditionalFormatting sqref="C897:C928">
     <cfRule type="duplicateValues" dxfId="132" priority="161"/>
     <cfRule type="duplicateValues" dxfId="131" priority="162"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C938:C940">
+  <conditionalFormatting sqref="C939:C941">
     <cfRule type="duplicateValues" dxfId="130" priority="1722"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C980 C982 C984 C986:C998 C1000 C1002:C1006 C1008:C1077">
+  <conditionalFormatting sqref="C981 C983 C985 C987:C999 C1001 C1003:C1007 C1009:C1078">
     <cfRule type="duplicateValues" dxfId="129" priority="8164"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C981 C983 C985 C941:C979 C689:C693 C687 C641 C928:C937 C698:C704 C706:C751 C655:C678 C876:C895 C753:C760 C574:C639 C806:C855 C777:C803 C470 C49:C180 C472 C474 C476 C479 C481 C483 C485 C487:C508 C7:C46">
+  <conditionalFormatting sqref="C982 C984 C986 C942:C980 C690:C694 C688 C642 C929:C938 C699:C705 C707:C752 C656:C679 C877:C896 C754:C761 C575:C640 C807:C856 C778:C804 C471 C50:C181 C473 C475 C477 C480 C482 C484 C486 C488:C509 C8:C47">
     <cfRule type="duplicateValues" dxfId="128" priority="14749"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1001">
+  <conditionalFormatting sqref="C1002">
     <cfRule type="duplicateValues" dxfId="127" priority="137"/>
     <cfRule type="duplicateValues" dxfId="126" priority="139"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1079:C1086">
+  <conditionalFormatting sqref="C1080:C1087">
     <cfRule type="duplicateValues" dxfId="125" priority="9753"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1087:C1088">
+  <conditionalFormatting sqref="C1088:C1089">
     <cfRule type="duplicateValues" dxfId="124" priority="103"/>
     <cfRule type="duplicateValues" dxfId="123" priority="104"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1089:C1242 C928:C1000 C706:C751 C876:C895 C753:C760 C1002:C1006 C1008:C1077 C695:C704 C1244 C574:C693 C806:C855 C777:C803 C1246:C1048576 C470 C49:C180 C472 C474 C476 C479 C481 C483 C485 C487:C508 C4:C46">
+  <conditionalFormatting sqref="C1090:C1243 C929:C1001 C707:C752 C877:C896 C754:C761 C1003:C1007 C1009:C1078 C696:C705 C1245 C575:C694 C807:C856 C778:C804 C1247:C1048576 C471 C50:C181 C473 C475 C477 C480 C482 C484 C486 C488:C509 C4:C47">
     <cfRule type="duplicateValues" dxfId="122" priority="14715"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1089:C1242 C1244 C1079:C1086 C806:C1077 C770:C803 C574:C767 C1246:C1048576 C470 C49:C180 C472 C474 C476 C479 C481 C483 C485 C487:C570 C4:C46">
+  <conditionalFormatting sqref="C1090:C1243 C1245 C1080:C1087 C807:C1078 C771:C804 C575:C768 C1247:C1048576 C471 C50:C181 C473 C475 C477 C480 C482 C484 C486 C488:C571 C4:C47">
     <cfRule type="duplicateValues" dxfId="121" priority="14747"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1090">
+  <conditionalFormatting sqref="C1091">
     <cfRule type="duplicateValues" dxfId="120" priority="256"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1091 C1093 C1095 C1097 C1099 C1101">
+  <conditionalFormatting sqref="C1092 C1094 C1096 C1098 C1100 C1102">
     <cfRule type="duplicateValues" dxfId="119" priority="255"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1091">
+  <conditionalFormatting sqref="C1092">
     <cfRule type="duplicateValues" dxfId="118" priority="254"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1145:C1146 C1128 C1089 C1103 C1107 C1109 C1111 C1113 C1115 C1117 C1119 C1121 C1123 C1125 C1130 C1132 C1134 C1136 C1138 C1140 C1142 C1148 C1150 C1152 C1154 C1156 C1158 C1160 C1162 C1164 C1166 C1168 C1170 C1172 C1174 C1105 C1176 C1179:C1242 C1244 C1246:C1048576">
+  <conditionalFormatting sqref="C1146:C1147 C1129 C1090 C1104 C1108 C1110 C1112 C1114 C1116 C1118 C1120 C1122 C1124 C1126 C1131 C1133 C1135 C1137 C1139 C1141 C1143 C1149 C1151 C1153 C1155 C1157 C1159 C1161 C1163 C1165 C1167 C1169 C1171 C1173 C1175 C1106 C1177 C1180:C1243 C1245 C1247:C1048576">
     <cfRule type="duplicateValues" dxfId="117" priority="312"/>
     <cfRule type="duplicateValues" dxfId="116" priority="858"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1147 C1106 C696 C1090 C1092 C1094 C1096 C1098 C1100 C1102 C1108 C1110 C1112 C1114 C1116 C1118 C1120 C1122 C1124 C1126:C1127 C1129 C1131 C1133 C1135 C1137 C1139 C1141 C1143:C1144 C1149 C1151 C1153 C1155 C1157 C1159 C1161 C1163 C1165 C1167 C1169 C1171 C1173 C1175 C1104 C1177:C1178">
+  <conditionalFormatting sqref="C1148 C1107 C697 C1091 C1093 C1095 C1097 C1099 C1101 C1103 C1109 C1111 C1113 C1115 C1117 C1119 C1121 C1123 C1125 C1127:C1128 C1130 C1132 C1134 C1136 C1138 C1140 C1142 C1144:C1145 C1150 C1152 C1154 C1156 C1158 C1160 C1162 C1164 C1166 C1168 C1170 C1172 C1174 C1176 C1105 C1178:C1179">
     <cfRule type="duplicateValues" dxfId="115" priority="1045"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1243 C1245">
+  <conditionalFormatting sqref="C1244 C1246">
     <cfRule type="duplicateValues" dxfId="114" priority="100"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1243">
+  <conditionalFormatting sqref="C1244">
     <cfRule type="duplicateValues" dxfId="113" priority="98"/>
     <cfRule type="duplicateValues" dxfId="112" priority="99"/>
     <cfRule type="duplicateValues" dxfId="111" priority="101"/>
@@ -9827,184 +9846,184 @@
     <cfRule type="duplicateValues" dxfId="107" priority="15"/>
     <cfRule type="duplicateValues" dxfId="106" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D9">
+  <conditionalFormatting sqref="D5:D10">
     <cfRule type="duplicateValues" dxfId="105" priority="178"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D54:D63">
+  <conditionalFormatting sqref="D55:D64">
     <cfRule type="duplicateValues" dxfId="104" priority="53"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D64:D78">
+  <conditionalFormatting sqref="D65:D79">
     <cfRule type="duplicateValues" dxfId="103" priority="13557"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D479">
+  <conditionalFormatting sqref="D480">
     <cfRule type="duplicateValues" dxfId="102" priority="24"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D506">
+  <conditionalFormatting sqref="D507">
     <cfRule type="duplicateValues" dxfId="101" priority="112"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D524:D525 D548 D517:D519 D507:D512">
+  <conditionalFormatting sqref="D525:D526 D549 D518:D520 D508:D513">
     <cfRule type="duplicateValues" dxfId="100" priority="8903"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D533:D538 D549 D543:D547 K776">
+  <conditionalFormatting sqref="D534:D539 D550 D544:D548 K777">
     <cfRule type="duplicateValues" dxfId="99" priority="9242"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D596">
+  <conditionalFormatting sqref="D597">
     <cfRule type="duplicateValues" dxfId="98" priority="224"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D597">
+  <conditionalFormatting sqref="D598">
     <cfRule type="duplicateValues" dxfId="97" priority="220"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D598">
+  <conditionalFormatting sqref="D599">
     <cfRule type="duplicateValues" dxfId="96" priority="222"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D599:D607">
+  <conditionalFormatting sqref="D600:D608">
     <cfRule type="duplicateValues" dxfId="95" priority="8562"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D640:D641">
+  <conditionalFormatting sqref="D641:D642">
     <cfRule type="duplicateValues" dxfId="94" priority="3559"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D642:D652">
+  <conditionalFormatting sqref="D643:D653">
     <cfRule type="duplicateValues" dxfId="93" priority="175"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D653:D654">
+  <conditionalFormatting sqref="D654:D655">
     <cfRule type="duplicateValues" dxfId="92" priority="174"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D666:D667">
+  <conditionalFormatting sqref="D667:D668">
     <cfRule type="duplicateValues" dxfId="91" priority="168"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D668">
+  <conditionalFormatting sqref="D669">
     <cfRule type="duplicateValues" dxfId="90" priority="144"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D675">
+  <conditionalFormatting sqref="D676">
     <cfRule type="duplicateValues" dxfId="89" priority="143"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D679">
+  <conditionalFormatting sqref="D680">
     <cfRule type="duplicateValues" dxfId="88" priority="170"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D681">
+  <conditionalFormatting sqref="D682">
     <cfRule type="duplicateValues" dxfId="87" priority="167"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D688">
+  <conditionalFormatting sqref="D689">
     <cfRule type="duplicateValues" dxfId="86" priority="186"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D691">
+  <conditionalFormatting sqref="D692">
     <cfRule type="duplicateValues" dxfId="85" priority="171"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D692:D693">
+  <conditionalFormatting sqref="D693:D694">
     <cfRule type="duplicateValues" dxfId="84" priority="172"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D695">
+  <conditionalFormatting sqref="D696">
     <cfRule type="duplicateValues" dxfId="83" priority="183"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D699:D704 D706:D723">
+  <conditionalFormatting sqref="D700:D705 D707:D724">
     <cfRule type="duplicateValues" dxfId="82" priority="6305"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D705">
+  <conditionalFormatting sqref="D706">
     <cfRule type="duplicateValues" dxfId="81" priority="158"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D727:D728">
+  <conditionalFormatting sqref="D728:D729">
     <cfRule type="duplicateValues" dxfId="80" priority="1883"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D729:D751 D753:D760">
+  <conditionalFormatting sqref="D730:D752 D754:D761">
     <cfRule type="duplicateValues" dxfId="79" priority="2135"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D752">
+  <conditionalFormatting sqref="D753">
     <cfRule type="duplicateValues" dxfId="78" priority="155"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D763">
+  <conditionalFormatting sqref="D764">
     <cfRule type="duplicateValues" dxfId="77" priority="118"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D764">
+  <conditionalFormatting sqref="D765">
     <cfRule type="duplicateValues" dxfId="76" priority="115"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D765:D767">
+  <conditionalFormatting sqref="D766:D768">
     <cfRule type="duplicateValues" dxfId="75" priority="121"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D777:D778">
+  <conditionalFormatting sqref="D778:D779">
     <cfRule type="duplicateValues" dxfId="74" priority="205"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D779">
+  <conditionalFormatting sqref="D780">
     <cfRule type="duplicateValues" dxfId="73" priority="201"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D780">
+  <conditionalFormatting sqref="D781">
     <cfRule type="duplicateValues" dxfId="72" priority="204"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D781">
+  <conditionalFormatting sqref="D782">
     <cfRule type="duplicateValues" dxfId="71" priority="203"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D782">
+  <conditionalFormatting sqref="D783">
     <cfRule type="duplicateValues" dxfId="70" priority="202"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D783:D784">
+  <conditionalFormatting sqref="D784:D785">
     <cfRule type="duplicateValues" dxfId="69" priority="206"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D806:D810 D785:D803">
+  <conditionalFormatting sqref="D807:D811 D786:D804">
     <cfRule type="duplicateValues" dxfId="68" priority="9936"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D826">
+  <conditionalFormatting sqref="D827">
     <cfRule type="duplicateValues" dxfId="67" priority="234"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D876:D880 D882:D889">
+  <conditionalFormatting sqref="D877:D881 D883:D890">
     <cfRule type="duplicateValues" dxfId="66" priority="232"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D881">
+  <conditionalFormatting sqref="D882">
     <cfRule type="duplicateValues" dxfId="65" priority="231"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D896:D927">
+  <conditionalFormatting sqref="D897:D928">
     <cfRule type="duplicateValues" dxfId="64" priority="163"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D938:D940">
+  <conditionalFormatting sqref="D939:D941">
     <cfRule type="duplicateValues" dxfId="63" priority="1723"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D941:D979 D47 D50:D51 D44:D45 D811:D812 D827:D834 D821:D825 D698 D608:D639 D689:D690 D724:D726 D680 D669:D674 D682:D687 D491:D505 D676:D678 D655:D665 D574:D595 D8:D12 D4">
+  <conditionalFormatting sqref="D942:D980 D48 D51:D52 D45:D46 D812:D813 D828:D835 D822:D826 D699 D609:D640 D690:D691 D725:D727 D681 D670:D675 D683:D688 D492:D506 D677:D679 D656:D666 D575:D596 D9:D13 D4">
     <cfRule type="duplicateValues" dxfId="62" priority="12220"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D981 D983 D985">
+  <conditionalFormatting sqref="D982 D984 D986">
     <cfRule type="duplicateValues" dxfId="61" priority="245"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1001">
+  <conditionalFormatting sqref="D1002">
     <cfRule type="duplicateValues" dxfId="60" priority="138"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1024">
+  <conditionalFormatting sqref="D1025">
     <cfRule type="duplicateValues" dxfId="59" priority="192"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1025:D1028 D980 D982 D984 D1000 D986:D998 D1032:D1077 D1008:D1023 D1002:D1006">
+  <conditionalFormatting sqref="D1026:D1029 D981 D983 D985 D1001 D987:D999 D1033:D1078 D1009:D1024 D1003:D1007">
     <cfRule type="duplicateValues" dxfId="58" priority="8154"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1029:D1030">
+  <conditionalFormatting sqref="D1030:D1031">
     <cfRule type="duplicateValues" dxfId="57" priority="2626"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1031">
+  <conditionalFormatting sqref="D1032">
     <cfRule type="duplicateValues" dxfId="56" priority="194"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1079">
+  <conditionalFormatting sqref="D1080">
     <cfRule type="duplicateValues" dxfId="55" priority="147"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1080:D1086">
+  <conditionalFormatting sqref="D1081:D1087">
     <cfRule type="duplicateValues" dxfId="54" priority="9754"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1087:D1088">
+  <conditionalFormatting sqref="D1088:D1089">
     <cfRule type="duplicateValues" dxfId="53" priority="105"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1090">
+  <conditionalFormatting sqref="D1091">
     <cfRule type="duplicateValues" dxfId="52" priority="258"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1212">
+  <conditionalFormatting sqref="D1213">
     <cfRule type="duplicateValues" dxfId="51" priority="130"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1213">
+  <conditionalFormatting sqref="D1214">
     <cfRule type="duplicateValues" dxfId="50" priority="133"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1214:D1227 D1197:D1211 D1186:D1188 D1089 D999 D696:D697 D1091:D1184 D1190:D1195 D1230:D1242 D1244:D1048576">
+  <conditionalFormatting sqref="D1215:D1228 D1198:D1212 D1187:D1189 D1090 D1000 D697:D698 D1092:D1185 D1191:D1196 D1231:D1243 D1245:D1048576">
     <cfRule type="duplicateValues" dxfId="49" priority="7226"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1228">
+  <conditionalFormatting sqref="D1229">
     <cfRule type="duplicateValues" dxfId="48" priority="129"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1229">
+  <conditionalFormatting sqref="D1230">
     <cfRule type="duplicateValues" dxfId="47" priority="128"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1243">
+  <conditionalFormatting sqref="D1244">
     <cfRule type="duplicateValues" dxfId="46" priority="102"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
@@ -10021,52 +10040,52 @@
     <cfRule type="duplicateValues" dxfId="37" priority="5"/>
     <cfRule type="duplicateValues" dxfId="36" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H853">
+  <conditionalFormatting sqref="H854">
     <cfRule type="duplicateValues" dxfId="35" priority="228"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H854">
+  <conditionalFormatting sqref="H855">
     <cfRule type="duplicateValues" dxfId="34" priority="227"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H855">
+  <conditionalFormatting sqref="H856">
     <cfRule type="duplicateValues" dxfId="33" priority="226"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H856:H864">
+  <conditionalFormatting sqref="H857:H865">
     <cfRule type="duplicateValues" dxfId="32" priority="8561"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H936:H938 H940 H942:H943">
+  <conditionalFormatting sqref="H937:H939 H941 H943:H944">
     <cfRule type="duplicateValues" dxfId="31" priority="166"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H939 H941">
+  <conditionalFormatting sqref="H940 H942">
     <cfRule type="duplicateValues" dxfId="30" priority="165"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H986">
+  <conditionalFormatting sqref="H987">
     <cfRule type="duplicateValues" dxfId="29" priority="242"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H987">
+  <conditionalFormatting sqref="H988">
     <cfRule type="duplicateValues" dxfId="28" priority="241"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H988">
+  <conditionalFormatting sqref="H989">
     <cfRule type="duplicateValues" dxfId="27" priority="240"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H989:H1067">
+  <conditionalFormatting sqref="H990:H1068">
     <cfRule type="duplicateValues" dxfId="26" priority="10291"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I890:I891">
+  <conditionalFormatting sqref="I891:I892">
     <cfRule type="duplicateValues" dxfId="25" priority="212"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I892">
+  <conditionalFormatting sqref="I893">
     <cfRule type="duplicateValues" dxfId="24" priority="208"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I893">
+  <conditionalFormatting sqref="I894">
     <cfRule type="duplicateValues" dxfId="23" priority="211"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I894">
+  <conditionalFormatting sqref="I895">
     <cfRule type="duplicateValues" dxfId="22" priority="210"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I895">
+  <conditionalFormatting sqref="I896">
     <cfRule type="duplicateValues" dxfId="21" priority="209"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I896:I911">
+  <conditionalFormatting sqref="I897:I912">
     <cfRule type="duplicateValues" dxfId="20" priority="5803"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>